<commit_message>
update report and rating
</commit_message>
<xml_diff>
--- a/BackEnd/files/report.xlsx
+++ b/BackEnd/files/report.xlsx
@@ -19,12 +19,144 @@
     <t>991000001799704574</t>
   </si>
   <si>
+    <t>991000364949704574</t>
+  </si>
+  <si>
+    <t>991000050149704574</t>
+  </si>
+  <si>
+    <t>991000220919704574</t>
+  </si>
+  <si>
+    <t>991000027049704574</t>
+  </si>
+  <si>
     <t>991000254419704574</t>
   </si>
   <si>
+    <t>991000202639704574</t>
+  </si>
+  <si>
+    <t>991000249439704574</t>
+  </si>
+  <si>
+    <t>991000112729704574</t>
+  </si>
+  <si>
+    <t>991000235819704574</t>
+  </si>
+  <si>
+    <t>991000072849704574</t>
+  </si>
+  <si>
+    <t>991000365019704574</t>
+  </si>
+  <si>
+    <t>991000050239704574</t>
+  </si>
+  <si>
+    <t>991000236569704574</t>
+  </si>
+  <si>
+    <t>991000239839704574</t>
+  </si>
+  <si>
+    <t>991000115259704574</t>
+  </si>
+  <si>
+    <t>991000601979704574</t>
+  </si>
+  <si>
+    <t>991000244649704574</t>
+  </si>
+  <si>
+    <t>991000661829704574</t>
+  </si>
+  <si>
+    <t>991000252139704574</t>
+  </si>
+  <si>
+    <t>991000329829704574</t>
+  </si>
+  <si>
+    <t>991001066317904574</t>
+  </si>
+  <si>
+    <t>991000240249704574</t>
+  </si>
+  <si>
+    <t>991000111799704574</t>
+  </si>
+  <si>
+    <t>991000250779704574</t>
+  </si>
+  <si>
+    <t>991000212849704574</t>
+  </si>
+  <si>
+    <t>991000364389704574</t>
+  </si>
+  <si>
+    <t>991000051099704574</t>
+  </si>
+  <si>
+    <t>991000247059704574</t>
+  </si>
+  <si>
+    <t>991000350969704574</t>
+  </si>
+  <si>
+    <t>991000067479704574</t>
+  </si>
+  <si>
+    <t>991000157529704574</t>
+  </si>
+  <si>
+    <t>991000257629704574</t>
+  </si>
+  <si>
+    <t>991000267479704574</t>
+  </si>
+  <si>
+    <t>991001070189604574</t>
+  </si>
+  <si>
+    <t>991000396619704574</t>
+  </si>
+  <si>
+    <t>991000084539704574</t>
+  </si>
+  <si>
+    <t>991000251609704574</t>
+  </si>
+  <si>
+    <t>991000364539704574</t>
+  </si>
+  <si>
+    <t>991000051309704574</t>
+  </si>
+  <si>
     <t>991000121389704574</t>
   </si>
   <si>
+    <t>991000383989704574</t>
+  </si>
+  <si>
+    <t>991000211589704574</t>
+  </si>
+  <si>
+    <t>991000107239704574</t>
+  </si>
+  <si>
+    <t>991000080409704574</t>
+  </si>
+  <si>
+    <t>991000399779704574</t>
+  </si>
+  <si>
+    <t>991000070059704574</t>
+  </si>
+  <si>
     <t>991000252329704574</t>
   </si>
   <si>
@@ -34,31 +166,7 @@
     <t>991000249599704574</t>
   </si>
   <si>
-    <t>991000080409704574</t>
-  </si>
-  <si>
-    <t>991000399779704574</t>
-  </si>
-  <si>
-    <t>991000257629704574</t>
-  </si>
-  <si>
-    <t>991000239839704574</t>
-  </si>
-  <si>
-    <t>991000249439704574</t>
-  </si>
-  <si>
-    <t>991000236569704574</t>
-  </si>
-  <si>
-    <t>991000115259704574</t>
-  </si>
-  <si>
-    <t>991000364949704574</t>
-  </si>
-  <si>
-    <t>991000050149704574</t>
+    <t>991000244239704574</t>
   </si>
   <si>
     <t>991000250179704574</t>
@@ -73,129 +181,129 @@
     <t>991000451839704574</t>
   </si>
   <si>
-    <t>991000329829704574</t>
-  </si>
-  <si>
-    <t>991000111799704574</t>
-  </si>
-  <si>
-    <t>991000244649704574</t>
-  </si>
-  <si>
-    <t>991000661829704574</t>
-  </si>
-  <si>
-    <t>991000112729704574</t>
-  </si>
-  <si>
-    <t>991000235819704574</t>
-  </si>
-  <si>
-    <t>991000072849704574</t>
-  </si>
-  <si>
-    <t>991000027049704574</t>
-  </si>
-  <si>
-    <t>991001070189604574</t>
-  </si>
-  <si>
-    <t>991000383989704574</t>
-  </si>
-  <si>
-    <t>991000211589704574</t>
-  </si>
-  <si>
-    <t>991000396619704574</t>
-  </si>
-  <si>
-    <t>991000084539704574</t>
-  </si>
-  <si>
-    <t>991000107239704574</t>
-  </si>
-  <si>
-    <t>991000212849704574</t>
-  </si>
-  <si>
-    <t>991000247059704574</t>
-  </si>
-  <si>
-    <t>991000244239704574</t>
-  </si>
-  <si>
-    <t>991000350969704574</t>
-  </si>
-  <si>
-    <t>991000067479704574</t>
-  </si>
-  <si>
-    <t>991000267479704574</t>
-  </si>
-  <si>
-    <t>991000365019704574</t>
-  </si>
-  <si>
-    <t>991000050239704574</t>
-  </si>
-  <si>
-    <t>991000220919704574</t>
+    <t>991001069871904574</t>
   </si>
   <si>
     <t>991001094844904574</t>
   </si>
   <si>
-    <t>991000252139704574</t>
-  </si>
-  <si>
-    <t>991000601979704574</t>
-  </si>
-  <si>
-    <t>991000070059704574</t>
-  </si>
-  <si>
-    <t>991000251609704574</t>
-  </si>
-  <si>
-    <t>991000364389704574</t>
-  </si>
-  <si>
-    <t>991000157529704574</t>
-  </si>
-  <si>
-    <t>991000051099704574</t>
-  </si>
-  <si>
-    <t>991000240249704574</t>
-  </si>
-  <si>
-    <t>991000202639704574</t>
-  </si>
-  <si>
-    <t>991000250779704574</t>
-  </si>
-  <si>
-    <t>991001066317904574</t>
-  </si>
-  <si>
-    <t>991000364539704574</t>
-  </si>
-  <si>
-    <t>991000051309704574</t>
-  </si>
-  <si>
-    <t>991001069871904574</t>
-  </si>
-  <si>
     <t xml:space="preserve">Love and sex after 60 </t>
   </si>
   <si>
+    <t>Dangerous men &amp; adventurous women</t>
+  </si>
+  <si>
+    <t>Transforming desire</t>
+  </si>
+  <si>
+    <t>The currency of Eros</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sex, dating, and love </t>
   </si>
   <si>
+    <t>"When the lamp is shattered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Love &amp; loss </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jane Austen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jane Austen and the war of ideas </t>
+  </si>
+  <si>
+    <t>Writing love</t>
+  </si>
+  <si>
+    <t>Critical tales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The road less traveled </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angels of September </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Northanger Abbey ; Lady Susan ; The Watsons ; and Sanditon </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Middlemarch </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erotic faith </t>
+  </si>
+  <si>
+    <t>Four complete novels /</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Free to love again </t>
+  </si>
+  <si>
+    <t>The Symposium ; and, The Phaedrus</t>
+  </si>
+  <si>
+    <t>Teenage couples. how to build a relationship that lasts / Caring, commitment, and change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dear God, kids rainbow </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Classical Hollywood comedy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Love and friendship </t>
+  </si>
+  <si>
+    <t>Medieval Latin and the rise of European love-lyric</t>
+  </si>
+  <si>
+    <t>The art of love</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jane Eyre </t>
+  </si>
+  <si>
+    <t>Catullan provocations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Of kings and poets </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I'd rather be married </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Be happy you are loved </t>
+  </si>
+  <si>
+    <t>Of chastity and power</t>
+  </si>
+  <si>
+    <t>Boston marriages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grandfather's journey </t>
+  </si>
+  <si>
+    <t>Rethinking The romance of the Rose</t>
+  </si>
+  <si>
     <t>The sacred and profane love machine</t>
   </si>
   <si>
+    <t>The Song of Eros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Elizabethan love sonnet </t>
+  </si>
+  <si>
+    <t>Letters to Margaret Gilcriest</t>
+  </si>
+  <si>
+    <t>Love and friendship in Plato and Aristotle</t>
+  </si>
+  <si>
     <t xml:space="preserve">The pursuit of love </t>
   </si>
   <si>
@@ -205,25 +313,7 @@
     <t xml:space="preserve">Creating love </t>
   </si>
   <si>
-    <t>Letters to Margaret Gilcriest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I'd rather be married </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Angels of September </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Love &amp; loss </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The road less traveled </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Northanger Abbey ; Lady Susan ; The Watsons ; and Sanditon </t>
-  </si>
-  <si>
-    <t>Dangerous men &amp; adventurous women</t>
+    <t xml:space="preserve">Getting the love you want </t>
   </si>
   <si>
     <t xml:space="preserve">Double-header </t>
@@ -238,136 +328,136 @@
     <t xml:space="preserve">Wizard and Wart </t>
   </si>
   <si>
-    <t>The Symposium ; and, The Phaedrus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Classical Hollywood comedy </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Erotic faith </t>
-  </si>
-  <si>
-    <t>Four complete novels /</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jane Austen </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jane Austen and the war of ideas </t>
-  </si>
-  <si>
-    <t>Writing love</t>
-  </si>
-  <si>
-    <t>The currency of Eros</t>
-  </si>
-  <si>
-    <t>Of chastity and power</t>
-  </si>
-  <si>
-    <t>The Song of Eros</t>
-  </si>
-  <si>
-    <t>Boston marriages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Elizabethan love sonnet </t>
-  </si>
-  <si>
-    <t>Medieval Latin and the rise of European love-lyric</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jane Eyre </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Getting the love you want </t>
-  </si>
-  <si>
-    <t>Catullan provocations</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Be happy you are loved </t>
-  </si>
-  <si>
-    <t>Critical tales</t>
-  </si>
-  <si>
-    <t>Transforming desire</t>
+    <t xml:space="preserve">Shamans and kushtakas </t>
   </si>
   <si>
     <t xml:space="preserve">The diary of a man of fifty </t>
   </si>
   <si>
-    <t xml:space="preserve">Free to love again </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Middlemarch </t>
-  </si>
-  <si>
-    <t>Love and friendship in Plato and Aristotle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Grandfather's journey </t>
-  </si>
-  <si>
-    <t>The art of love</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Of kings and poets </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dear God, kids rainbow </t>
-  </si>
-  <si>
-    <t>"When the lamp is shattered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Love and friendship </t>
-  </si>
-  <si>
-    <t>Teenage couples. how to build a relationship that lasts / Caring, commitment, and change</t>
-  </si>
-  <si>
-    <t>Rethinking The romance of the Rose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shamans and kushtakas </t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
     <t>['sex', 'instruction', 'older', 'people', 'love', 'age']</t>
   </si>
   <si>
+    <t>['love', 'stories', 'american', 'women', 'authors', 'readers', 'sex', 'role', 'literature']</t>
+  </si>
+  <si>
+    <t>['erotic', 'poetry', 'english', 'epic', 'desire', 'literature', 'love', 'sex']</t>
+  </si>
+  <si>
+    <t>['love', 'poetry', 'european', 'literature', 'women', 'sex', 'role']</t>
+  </si>
+  <si>
     <t>['dating', 'social', 'customs', 'love', 'sex']</t>
   </si>
   <si>
+    <t>['love', 'poetry', 'latin', 'psychoanalysis', 'literature', 'desire', 'narration', 'rhetoric', 'rome', 'ancient']</t>
+  </si>
+  <si>
+    <t>['love', 'stories', 'english', 'american', 'fiction']</t>
+  </si>
+  <si>
+    <t>['women', 'literature', 'love', 'stories', 'english']</t>
+  </si>
+  <si>
+    <t>['english', 'fiction', 'women', 'literature', 'love', 'stories']</t>
+  </si>
+  <si>
+    <t>['french', 'fiction', 'epistolary', 'love', 'stories', 'women', 'literature', 'letters']</t>
+  </si>
+  <si>
+    <t>['women', 'literature', 'love', 'stories', 'french', 'characters', 'characteristics', 'rhetoric', 'literary', 'form']</t>
+  </si>
+  <si>
+    <t>['self', 'actualization', 'psychology', 'maturation', 'interpersonal', 'relations', 'love', 'values', 'spirituality']</t>
+  </si>
+  <si>
+    <t>['love', 'stories', 'detective', 'mystery']</t>
+  </si>
+  <si>
+    <t>['horror', 'tales', 'books', 'reading', 'love', 'stories', 'english']</t>
+  </si>
+  <si>
+    <t>['english', 'city', 'town', 'life', 'married', 'people', 'young', 'women']</t>
+  </si>
+  <si>
+    <t>['english', 'fiction', 'love', 'stories', 'literature']</t>
+  </si>
+  <si>
+    <t>['literature', 'historical', 'fiction', 'love', 'stories']</t>
+  </si>
+  <si>
+    <t>['sex', 'christian', 'life']</t>
+  </si>
+  <si>
+    <t>['love', 'soul', 'rhetoric', 'ancient']</t>
+  </si>
+  <si>
+    <t>['man', 'woman', 'relationships', 'teenagers', 'love', 'mate', 'selection', 'family', 'marriage', 'sociology', 'social', 'history', 'sciences']</t>
+  </si>
+  <si>
+    <t>['god', 'christianity', 'providence', 'government', 'color', 'early', 'childhood', 'education', 'children', 'stories']</t>
+  </si>
+  <si>
+    <t>['comedy', 'films', 'love', 'motion', 'pictures']</t>
+  </si>
+  <si>
+    <t>['love', 'literature', 'european', 'friendship']</t>
+  </si>
+  <si>
+    <t>['love', 'poetry', 'european', 'latin', 'medieval', 'modern']</t>
+  </si>
+  <si>
+    <t>['courtly', 'love', 'literature', 'poetry', 'latin', 'medieval', 'modern']</t>
+  </si>
+  <si>
+    <t>['governesses', 'fathers', 'daughters', 'mentally', 'ill', 'women', 'charity', 'schools', 'married', 'people', 'country', 'homes', 'young', 'orphans']</t>
+  </si>
+  <si>
+    <t>['verse', 'satire', 'latin', 'love', 'epigrams']</t>
+  </si>
+  <si>
+    <t>['spanish', 'poetry', 'courtly', 'love', 'literature', 'authors', 'patrons']</t>
+  </si>
+  <si>
+    <t>['mate', 'selection', 'man', 'woman', 'relationships', 'dating', 'social', 'customs', 'love']</t>
+  </si>
+  <si>
+    <t>['god', 'love', 'self', 'esteem', 'large', 'type', 'books']</t>
+  </si>
+  <si>
+    <t>['chastity', 'literature', 'english', 'feminism', 'kings', 'rulers', 'social', 'sciences', 'queens', 'sex', 'role', 'single', 'women']</t>
+  </si>
+  <si>
+    <t>['lesbian', 'couples', 'platonic', 'love']</t>
+  </si>
+  <si>
+    <t>['grandfathers', 'caldecott', 'medal', 'voyages', 'travels', 'homesickness', 'early', 'childhood', 'education', 'children', 'stories', 'social', 'issues', 'japanese', 'americans']</t>
+  </si>
+  <si>
+    <t>['love', 'poetry', 'french', 'literature', 'medieval', 'romances', 'manuscripts', 'courtly']</t>
+  </si>
+  <si>
     <t>['man', 'woman', 'relationships', 'married', 'people']</t>
   </si>
   <si>
+    <t>['love', 'poetry', 'greek']</t>
+  </si>
+  <si>
+    <t>['sonnets', 'english', 'poetry', 'love']</t>
+  </si>
+  <si>
+    <t>['world', 'war', 'authors', 'welsh', 'soldiers', 'love', 'letters']</t>
+  </si>
+  <si>
+    <t>['love', 'friendship']</t>
+  </si>
+  <si>
     <t>['love']</t>
   </si>
   <si>
-    <t>['world', 'war', 'authors', 'welsh', 'soldiers', 'love', 'letters']</t>
-  </si>
-  <si>
-    <t>['mate', 'selection', 'man', 'woman', 'relationships', 'dating', 'social', 'customs', 'love']</t>
-  </si>
-  <si>
-    <t>['love', 'stories', 'detective', 'mystery']</t>
-  </si>
-  <si>
-    <t>['love', 'stories', 'english', 'american', 'fiction']</t>
-  </si>
-  <si>
-    <t>['self', 'actualization', 'psychology', 'maturation', 'interpersonal', 'relations', 'love', 'values', 'spirituality']</t>
-  </si>
-  <si>
-    <t>['horror', 'tales', 'books', 'reading', 'love', 'stories', 'english']</t>
-  </si>
-  <si>
-    <t>['love', 'stories', 'american', 'women', 'authors', 'readers', 'sex', 'role', 'literature']</t>
+    <t>['marriage', 'love']</t>
   </si>
   <si>
     <t>['monsters', 'baseball', 'early', 'childhood', 'education', 'children', 'stories']</t>
@@ -382,133 +472,133 @@
     <t>['wizards', 'magic', 'animals', 'witchcraft', 'early', 'childhood', 'education', 'children', 'stories']</t>
   </si>
   <si>
-    <t>['love', 'soul', 'rhetoric', 'ancient']</t>
-  </si>
-  <si>
-    <t>['comedy', 'films', 'love', 'motion', 'pictures']</t>
-  </si>
-  <si>
-    <t>['english', 'fiction', 'love', 'stories', 'literature']</t>
-  </si>
-  <si>
-    <t>['literature', 'historical', 'fiction', 'love', 'stories']</t>
-  </si>
-  <si>
-    <t>['women', 'literature', 'love', 'stories', 'english']</t>
-  </si>
-  <si>
-    <t>['english', 'fiction', 'women', 'literature', 'love', 'stories']</t>
-  </si>
-  <si>
-    <t>['french', 'fiction', 'epistolary', 'love', 'stories', 'women', 'literature', 'letters']</t>
-  </si>
-  <si>
-    <t>['love', 'poetry', 'european', 'literature', 'women', 'sex', 'role']</t>
-  </si>
-  <si>
-    <t>['chastity', 'literature', 'english', 'feminism', 'kings', 'rulers', 'social', 'sciences', 'queens', 'sex', 'role', 'single', 'women']</t>
-  </si>
-  <si>
-    <t>['love', 'poetry', 'greek']</t>
-  </si>
-  <si>
-    <t>['lesbian', 'couples', 'platonic', 'love']</t>
-  </si>
-  <si>
-    <t>['sonnets', 'english', 'poetry', 'love']</t>
-  </si>
-  <si>
-    <t>['love', 'poetry', 'european', 'latin', 'medieval', 'modern']</t>
-  </si>
-  <si>
-    <t>['governesses', 'fathers', 'daughters', 'mentally', 'ill', 'women', 'charity', 'schools', 'married', 'people', 'country', 'homes', 'young', 'orphans']</t>
-  </si>
-  <si>
-    <t>['marriage', 'love']</t>
-  </si>
-  <si>
-    <t>['verse', 'satire', 'latin', 'love', 'epigrams']</t>
-  </si>
-  <si>
-    <t>['god', 'love', 'self', 'esteem', 'large', 'type', 'books']</t>
-  </si>
-  <si>
-    <t>['women', 'literature', 'love', 'stories', 'french', 'characters', 'characteristics', 'rhetoric', 'literary', 'form']</t>
-  </si>
-  <si>
-    <t>['erotic', 'poetry', 'english', 'epic', 'desire', 'literature', 'love', 'sex']</t>
+    <t>['tlingit', 'indians', 'haida', 'mythology', 'ethnic', 'race', 'studies', 'gender', 'social', 'sciences']</t>
   </si>
   <si>
     <t>['aging']</t>
   </si>
   <si>
-    <t>['sex', 'christian', 'life']</t>
-  </si>
-  <si>
-    <t>['english', 'city', 'town', 'life', 'married', 'people', 'young', 'women']</t>
-  </si>
-  <si>
-    <t>['love', 'friendship']</t>
-  </si>
-  <si>
-    <t>['grandfathers', 'caldecott', 'medal', 'voyages', 'travels', 'homesickness', 'early', 'childhood', 'education', 'children', 'stories', 'social', 'issues', 'japanese', 'americans']</t>
-  </si>
-  <si>
-    <t>['courtly', 'love', 'literature', 'poetry', 'latin', 'medieval', 'modern']</t>
-  </si>
-  <si>
-    <t>['spanish', 'poetry', 'courtly', 'love', 'literature', 'authors', 'patrons']</t>
-  </si>
-  <si>
-    <t>['god', 'christianity', 'providence', 'government', 'color', 'early', 'childhood', 'education', 'children', 'stories']</t>
-  </si>
-  <si>
-    <t>['love', 'poetry', 'latin', 'psychoanalysis', 'literature', 'desire', 'narration', 'rhetoric', 'rome', 'ancient']</t>
-  </si>
-  <si>
-    <t>['love', 'literature', 'european', 'friendship']</t>
-  </si>
-  <si>
-    <t>['man', 'woman', 'relationships', 'teenagers', 'love', 'mate', 'selection', 'family', 'marriage', 'sociology', 'social', 'history', 'sciences']</t>
-  </si>
-  <si>
-    <t>['love', 'poetry', 'french', 'literature', 'medieval', 'romances', 'manuscripts', 'courtly']</t>
-  </si>
-  <si>
-    <t>['tlingit', 'indians', 'haida', 'mythology', 'ethnic', 'race', 'studies', 'gender', 'social', 'sciences']</t>
-  </si>
-  <si>
     <t>['dXHAyncBufXmZs9o45Vl', 'dnHAyncBufXmZs9o45Vt', 'enHAyncBufXmZs9o45WS', 'eHHAyncBufXmZs9o45WA', 'eXHAyncBufXmZs9o45WJ', 'enHAyncBufXmZs9o45WS', 'b3HAyncBufXmZs9o45Ux']</t>
   </si>
   <si>
+    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['american', 'American', 'American_English', 'American_language'], ['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['authors', 'writer', 'author', 'generator', 'source'], ['readers', 'reader', 'subscriber', 'reviewer', 'referee', 'proofreader', 'lector', 'lecturer'], ['sex', 'sexual_activity', 'sexual_practice', 'sex_activity', 'sexual_urge', 'gender', 'sexuality', 'arouse', 'excite', 'turn_on', 'wind_up'], ['role', 'function', 'office', 'part', 'character', 'theatrical_role', 'persona', 'purpose', 'use'], ['literature', 'lit']]</t>
+  </si>
+  <si>
+    <t>[['erotic', 'titillating'], ['poetry', 'poesy', 'verse'], ['english', 'English', 'English_language', 'English_people', 'side'], ['epic', 'epic_poem', 'heroic_poem', 'epos', 'heroic', 'larger-than-life', 'epical'], ['desire', 'want', 'hope', 'trust'], ['literature', 'lit'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['sex', 'sexual_activity', 'sexual_practice', 'sex_activity', 'sexual_urge', 'gender', 'sexuality', 'arouse', 'excite', 'turn_on', 'wind_up']]</t>
+  </si>
+  <si>
+    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['poetry', 'poesy', 'verse'], ['european', 'European'], ['literature', 'lit'], ['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['sex', 'sexual_activity', 'sexual_practice', 'sex_activity', 'sexual_urge', 'gender', 'sexuality', 'arouse', 'excite', 'turn_on', 'wind_up'], ['role', 'function', 'office', 'part', 'character', 'theatrical_role', 'persona', 'purpose', 'use']]</t>
+  </si>
+  <si>
     <t>[['dating', 'geological_dating', 'date', 'date_stamp', 'go_steady', 'go_out', 'see'], ['social', 'sociable', 'mixer', 'societal'], ['customs', 'customs_duty', 'custom', 'impost', 'usage', 'usance', 'tradition'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['sex', 'sexual_activity', 'sexual_practice', 'sex_activity', 'sexual_urge', 'gender', 'sexuality', 'arouse', 'excite', 'turn_on', 'wind_up']]</t>
   </si>
   <si>
+    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['poetry', 'poesy', 'verse'], ['latin', 'Latin', 'Romance'], ['psychoanalysis', 'analysis', 'depth_psychology'], ['literature', 'lit'], ['desire', 'want', 'hope', 'trust'], ['narration', 'narrative', 'story', 'tale', 'recital', 'yarn'], ['rhetoric', 'grandiosity', 'magniloquence', 'ornateness', 'grandiloquence', 'palaver', 'hot_air', 'empty_words', 'empty_talk'], ['rome', 'Rome', 'Roma', 'Eternal_City', 'Italian_capital', 'capital_of_Italy'], ['ancient', 'antediluvian']]</t>
+  </si>
+  <si>
+    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['english', 'English', 'English_language', 'English_people', 'side'], ['american', 'American', 'American_English', 'American_language'], ['fiction', 'fabrication', 'fable']]</t>
+  </si>
+  <si>
+    <t>[['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['literature', 'lit'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['english', 'English', 'English_language', 'English_people', 'side']]</t>
+  </si>
+  <si>
+    <t>[['english', 'English', 'English_language', 'English_people', 'side'], ['fiction', 'fabrication', 'fable'], ['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['literature', 'lit'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle']]</t>
+  </si>
+  <si>
+    <t>[['french', 'French', 'French_people', 'Daniel_Chester_French', 'Gallic'], ['fiction', 'fabrication', 'fable'], ['epistolary', 'epistolatory'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['literature', 'lit'], ['letters', 'letter', 'missive', 'letter_of_the_alphabet', 'alphabetic_character', 'varsity_letter']]</t>
+  </si>
+  <si>
+    <t>[['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['literature', 'lit'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['french', 'French', 'French_people', 'Daniel_Chester_French', 'Gallic'], ['characters', 'fictional_character', 'fictitious_character', 'character', 'quality', 'lineament', 'fiber', 'fibre', 'role', 'theatrical_role', 'part', 'persona', 'eccentric', 'type', 'case', 'reference', 'character_reference', 'grapheme', 'graphic_symbol'], ['characteristics', 'feature', 'characteristic', 'device_characteristic'], ['narration', 'narrative', 'story', 'tale', 'recital', 'yarn'], ['rhetoric', 'grandiosity', 'magniloquence', 'ornateness', 'grandiloquence', 'palaver', 'hot_air', 'empty_words', 'empty_talk'], ['literary'], ['classes', 'class', 'category', 'family', 'form', 'grade', 'course', 'stratum', 'social_class', 'socio-economic_class', 'course_of_study', 'course_of_instruction', 'division', 'year', 'classify', 'sort', 'assort', 'sort_out', 'separate']]</t>
+  </si>
+  <si>
+    <t>[['self', 'ego'], ['actualization', 'realization', 'realisation', 'actualisation'], ['psychology', 'psychological_science'], ['maturation', 'ripening', 'maturement', 'growth', 'growing', 'development', 'ontogeny', 'ontogenesis', 'festering', 'suppuration'], ['interpersonal'], ['relations', 'dealings', 'relation', 'sexual_intercourse', 'intercourse', 'sex_act', 'copulation', 'coitus', 'coition', 'sexual_congress', 'congress', 'sexual_relation', 'carnal_knowledge', 'relative', 'telling', 'recounting', 'relation_back'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['values', 'value', 'economic_value', 'time_value', 'note_value', 'prize', 'treasure', 'appreciate', 'respect', 'esteem', 'prise', 'measure', 'evaluate', 'valuate', 'assess', 'appraise', 'rate'], ['spirituality', 'spiritualty', 'church_property', 'spiritualism', 'spiritism', 'otherworldliness']]</t>
+  </si>
+  <si>
+    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['detective', 'investigator', 'tec', 'police_detective'], ['mystery', 'enigma', 'secret', 'closed_book', 'mystery_story', 'whodunit']]</t>
+  </si>
+  <si>
+    <t>[['horror', 'repugnance', 'repulsion', 'revulsion'], ['tales', 'narrative', 'narration', 'story', 'tale', 'fib', 'tarradiddle', 'taradiddle'], ['books', 'book', 'volume', 'record', 'record_book', 'script', 'playscript', 'ledger', 'leger', 'account_book', 'book_of_account', 'rule_book', 'Koran', 'Quran', "al-Qur'an", 'Book', 'Bible', 'Christian_Bible', 'Good_Book', 'Holy_Scripture', 'Holy_Writ', 'Scripture', 'Word_of_God', 'Word', 'reserve', 'hold'], ['reading', 'meter_reading', 'indication', 'reading_material', 'interpretation', 'version', 'Reading', 'recitation', 'recital', 'read', 'say', 'scan', 'take', 'learn', 'study', 'register', 'show', 'record', 'understand', 'interpret', 'translate'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['english', 'English', 'English_language', 'English_people', 'side']]</t>
+  </si>
+  <si>
+    <t>[['english', 'English', 'English_language', 'English_people', 'side'], ['city', 'metropolis', 'urban_center'], ['town', 'townspeople', 'townsfolk', 'township', 'Town', 'Ithiel_Town'], ['life', 'living', 'animation', 'aliveness', 'lifetime', 'life-time', 'lifespan', 'liveliness', 'spirit', 'sprightliness', 'biography', 'life_story', 'life_history', 'life_sentence'], ['married', 'marry', 'get_married', 'wed', 'conjoin', 'hook_up_with', 'get_hitched_with', 'espouse', 'tie', 'splice', 'marital', 'matrimonial'], ['people', 'citizenry', 'multitude', 'masses', 'mass', 'hoi_polloi', 'the_great_unwashed'], ['youth', 'young_person', 'younker', 'spring_chicken', 'young', 'early_days', 'youthfulness', 'juvenility'], ['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex']]</t>
+  </si>
+  <si>
+    <t>[['english', 'English', 'English_language', 'English_people', 'side'], ['fiction', 'fabrication', 'fable'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['literature', 'lit']]</t>
+  </si>
+  <si>
+    <t>[['literature', 'lit'], ['historical', 'historic', 'diachronic'], ['fiction', 'fabrication', 'fable'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle']]</t>
+  </si>
+  <si>
+    <t>[['sex', 'sexual_activity', 'sexual_practice', 'sex_activity', 'sexual_urge', 'gender', 'sexuality', 'arouse', 'excite', 'turn_on', 'wind_up'], ['christian', 'Christian'], ['life', 'living', 'animation', 'aliveness', 'lifetime', 'life-time', 'lifespan', 'liveliness', 'spirit', 'sprightliness', 'biography', 'life_story', 'life_history', 'life_sentence']]</t>
+  </si>
+  <si>
+    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['soul', 'psyche', 'person', 'individual', 'someone', 'somebody', 'mortal', 'soulfulness'], ['rhetoric', 'grandiosity', 'magniloquence', 'ornateness', 'grandiloquence', 'palaver', 'hot_air', 'empty_words', 'empty_talk'], ['ancient', 'antediluvian']]</t>
+  </si>
+  <si>
+    <t>[['man', 'adult_male', 'serviceman', 'military_man', 'military_personnel', 'homo', 'human_being', 'human', 'valet', 'valet_de_chambre', 'gentleman', "gentleman's_gentleman", 'Man', 'Isle_of_Man', 'piece', 'world', 'human_race', 'humanity', 'humankind', 'human_beings', 'humans', 'mankind'], ['woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['relationships', 'relationship', 'human_relationship', 'kinship', 'family_relationship'], ['teenagers', 'adolescent', 'stripling', 'teenager', 'teen'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['couples', 'couple', 'twosome', 'duo', 'duet', 'mates', 'match', 'pair', 'twain', 'brace', 'span', 'yoke', 'couplet', 'distich', 'dyad', 'duad', 'mate', 'twin', 'couple_on', 'couple_up', 'pair_off', 'partner_off', 'copulate'], ['selection', 'choice', 'option', 'pick', 'survival', 'survival_of_the_fittest', 'natural_selection', 'excerpt', 'excerption', 'extract'], ['household', 'family', 'house', 'home', 'menage'], ['marriage', 'matrimony', 'union', 'spousal_relationship', 'wedlock', 'married_couple', 'man_and_wife', 'wedding', 'marriage_ceremony'], ['sociology'], ['social', 'sociable', 'mixer', 'societal'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['sciences', 'science', 'scientific_discipline', 'skill']]</t>
+  </si>
+  <si>
+    <t>[['old', 'older', 'erstwhile', 'former', 'onetime', 'one-time', 'quondam', 'sometime', 'honest-to-god', 'honest-to-goodness', 'sure-enough', 'Old', 'previous'], ['christianity', 'Christianity', 'Christian_religion', 'Christendom'], ['providence', 'Providence', 'capital_of_Rhode_Island'], ['government', 'authorities', 'regime', 'governing', 'governance', 'government_activity', 'administration', 'politics', 'political_science'], ['color', 'colour', 'coloring', 'colouring', 'vividness', 'coloration', 'colouration', 'people_of_color', 'people_of_colour', 'semblance', 'gloss', 'coloring_material', 'colouring_material', 'colorize', 'colorise', 'colourise', 'colourize', 'color_in', 'colour_in', 'tinge', 'distort', 'emblazon', 'discolor', 'discolour'], ['early', 'former', 'other', 'early_on', 'ahead_of_time', 'too_soon', 'betimes'], ['childhood', 'puerility'], ['instruction', 'direction', 'education', 'teaching', 'pedagogy', 'didactics', 'educational_activity', 'command', 'statement', 'program_line'], ['children', 'child', 'kid', 'youngster', 'minor', 'shaver', 'nipper', 'small_fry', 'tiddler', 'tike', 'tyke', 'fry', 'nestling', 'baby'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle']]</t>
+  </si>
+  <si>
+    <t>[['comedy', 'drollery', 'clowning', 'funniness'], ['films', 'movie', 'film', 'picture', 'moving_picture', 'moving-picture_show', 'motion_picture', 'motion-picture_show', 'picture_show', 'pic', 'flick', 'cinema', 'celluloid', 'photographic_film', 'plastic_film', 'shoot', 'take'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['motion', 'gesture', 'movement', 'move', 'motility', 'question', 'apparent_motion', 'apparent_movement', 'gesticulate'], ['pictures', 'picture', 'image', 'icon', 'ikon', 'painting', 'mental_picture', 'impression', 'scene', 'pictorial_matter', 'movie', 'film', 'moving_picture', 'moving-picture_show', 'motion_picture', 'motion-picture_show', 'picture_show', 'pic', 'flick', 'video', 'word_picture', 'word-painting', 'delineation', 'depiction', 'characterization', 'characterisation', 'photograph', 'photo', 'exposure', 'visualize', 'visualise', 'envision', 'project', 'fancy', 'see', 'figure', 'depict', 'render', 'show']]</t>
+  </si>
+  <si>
+    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['literature', 'lit'], ['european', 'European'], ['friendship', 'friendly_relationship']]</t>
+  </si>
+  <si>
+    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['poetry', 'poesy', 'verse'], ['european', 'European'], ['latin', 'Latin', 'Romance'], ['medieval', 'mediaeval', 'gothic', 'chivalric', 'knightly'], ['modern', 'modern_font', 'Bodoni', 'Bodoni_font', 'mod', 'modernistic', 'advanced', 'forward-looking', 'innovative', 'Modern', 'New']]</t>
+  </si>
+  <si>
+    <t>[['courtly', 'formal', 'stately'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['literature', 'lit'], ['poetry', 'poesy', 'verse'], ['latin', 'Latin', 'Romance'], ['medieval', 'mediaeval', 'gothic', 'chivalric', 'knightly'], ['modern', 'modern_font', 'Bodoni', 'Bodoni_font', 'mod', 'modernistic', 'advanced', 'forward-looking', 'innovative', 'Modern', 'New']]</t>
+  </si>
+  <si>
+    <t>[['governesses', 'governess', 'regulate', 'regularize', 'regularise', 'order', 'govern', 'rule'], ['fathers', 'father', 'male_parent', 'begetter', 'forefather', 'sire', 'Father', 'Padre', 'Church_Father', 'Father_of_the_Church', 'Father-God', 'Fatherhood', 'founder', 'beginner', 'founding_father', 'don', 'beget', 'get', 'engender', 'mother', 'generate', 'bring_forth'], ['daughters', 'daughter', 'girl'], ['mentally'], ['ill', 'ailment', 'complaint', 'sick', 'inauspicious', 'ominous', 'badly', 'poorly'], ['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['charity', 'brotherly_love', "Jacob's_ladder", 'Greek_valerian', 'Polemonium_caeruleum', 'Polemonium_van-bruntiae', 'Polymonium_caeruleum_van-bruntiae'], ['schools', 'school', 'schoolhouse', 'schooling', 'schooltime', 'school_day', 'shoal', 'educate', 'train', 'cultivate', 'civilize', 'civilise'], ['married', 'marry', 'get_married', 'wed', 'conjoin', 'hook_up_with', 'get_hitched_with', 'espouse', 'tie', 'splice', 'marital', 'matrimonial'], ['people', 'citizenry', 'multitude', 'masses', 'mass', 'hoi_polloi', 'the_great_unwashed'], ['country', 'state', 'nation', 'land', 'commonwealth', 'res_publica', 'body_politic', 'rural_area', 'area'], ['homes', 'home', 'place', 'dwelling', 'domicile', 'abode', 'habitation', 'dwelling_house', 'home_plate', 'home_base', 'plate', 'base', 'family', 'household', 'house', 'menage', 'nursing_home', 'rest_home'], ['youth', 'young_person', 'younker', 'spring_chicken', 'young', 'early_days', 'youthfulness', 'juvenility'], ['orphans', 'orphan']]</t>
+  </si>
+  <si>
+    <t>[['poetry', 'poesy', 'verse'], ['satire', 'sarcasm', 'irony', 'caustic_remark'], ['latin', 'Latin', 'Romance'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['poetry', 'poesy', 'verse'], ['epigrams', 'epigram', 'quip']]</t>
+  </si>
+  <si>
+    <t>[['spanish', 'Spanish', 'Spanish_people'], ['poetry', 'poesy', 'verse'], ['courtly', 'formal', 'stately'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['literature', 'lit'], ['authors', 'writer', 'author', 'generator', 'source'], ['patrons', 'patron', 'frequenter', 'sponsor', 'supporter']]</t>
+  </si>
+  <si>
+    <t>[['couples', 'couple', 'twosome', 'duo', 'duet', 'mates', 'match', 'pair', 'twain', 'brace', 'span', 'yoke', 'couplet', 'distich', 'dyad', 'duad', 'mate', 'twin', 'couple_on', 'couple_up', 'pair_off', 'partner_off', 'copulate'], ['selection', 'choice', 'option', 'pick', 'survival', 'survival_of_the_fittest', 'natural_selection', 'excerpt', 'excerption', 'extract'], ['man', 'adult_male', 'serviceman', 'military_man', 'military_personnel', 'homo', 'human_being', 'human', 'valet', 'valet_de_chambre', 'gentleman', "gentleman's_gentleman", 'Man', 'Isle_of_Man', 'piece', 'world', 'human_race', 'humanity', 'humankind', 'human_beings', 'humans', 'mankind'], ['woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['relationships', 'relationship', 'human_relationship', 'kinship', 'family_relationship'], ['dating', 'geological_dating', 'date', 'date_stamp', 'go_steady', 'go_out', 'see'], ['social', 'sociable', 'mixer', 'societal'], ['customs', 'customs_duty', 'custom', 'impost', 'usage', 'usance', 'tradition'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk']]</t>
+  </si>
+  <si>
+    <t>[['old', 'older', 'erstwhile', 'former', 'onetime', 'one-time', 'quondam', 'sometime', 'honest-to-god', 'honest-to-goodness', 'sure-enough', 'Old', 'previous'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['self', 'ego'], ['values', 'value', 'economic_value', 'time_value', 'note_value', 'prize', 'treasure', 'appreciate', 'respect', 'esteem', 'prise', 'measure', 'evaluate', 'valuate', 'assess', 'appraise', 'rate'], ['large', 'big', 'bombastic', 'declamatory', 'orotund', 'tumid', 'turgid', 'magnanimous', 'prominent', 'enceinte', 'expectant', 'gravid', 'great', 'heavy', 'with_child', 'boastfully', 'vauntingly'], ['characters', 'fictional_character', 'fictitious_character', 'character', 'quality', 'lineament', 'fiber', 'fibre', 'role', 'theatrical_role', 'part', 'persona', 'eccentric', 'type', 'case', 'reference', 'character_reference', 'grapheme', 'graphic_symbol'], ['books', 'book', 'volume', 'record', 'record_book', 'script', 'playscript', 'ledger', 'leger', 'account_book', 'book_of_account', 'rule_book', 'Koran', 'Quran', "al-Qur'an", 'Book', 'Bible', 'Christian_Bible', 'Good_Book', 'Holy_Scripture', 'Holy_Writ', 'Scripture', 'Word_of_God', 'Word', 'reserve', 'hold']]</t>
+  </si>
+  <si>
+    <t>[['chastity', 'celibacy', 'sexual_abstention', 'virtue', 'sexual_morality'], ['literature', 'lit'], ['english', 'English', 'English_language', 'English_people', 'side'], ['feminism', 'feminist_movement', "women's_liberation_movement", "women's_lib"], ['kings', 'king', 'male_monarch', 'Rex', 'queen', 'world-beater', 'baron', 'big_businessman', 'business_leader', 'magnate', 'mogul', 'power', 'top_executive', 'tycoon', 'King', 'Billie_Jean_King', 'Billie_Jean_Moffitt_King', 'B._B._King', 'Riley_B_King', 'Martin_Luther_King', 'Martin_Luther_King_Jr.'], ['rulers', 'ruler', 'swayer', 'rule'], ['kings', 'king', 'male_monarch', 'Rex', 'queen', 'world-beater', 'baron', 'big_businessman', 'business_leader', 'magnate', 'mogul', 'power', 'top_executive', 'tycoon', 'King', 'Billie_Jean_King', 'Billie_Jean_Moffitt_King', 'B._B._King', 'Riley_B_King', 'Martin_Luther_King', 'Martin_Luther_King_Jr.'], ['social', 'sociable', 'mixer', 'societal'], ['sciences', 'science', 'scientific_discipline', 'skill'], ['queens', 'Queens', 'queen', 'queen_regnant', 'female_monarch', 'king', 'world-beater', 'fagot', 'faggot', 'fag', 'fairy', 'nance', 'pansy', 'queer', 'poof', 'poove', 'pouf', 'queen_mole_rat', 'tabby'], ['sex', 'sexual_activity', 'sexual_practice', 'sex_activity', 'sexual_urge', 'gender', 'sexuality', 'arouse', 'excite', 'turn_on', 'wind_up'], ['role', 'function', 'office', 'part', 'character', 'theatrical_role', 'persona', 'purpose', 'use'], ['single', 'bingle', 'one', '1', 'I', 'ace', 'unity', 'individual', 'unmarried', 'undivided', 'exclusive'], ['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex']]</t>
+  </si>
+  <si>
+    <t>[['lesbian', 'tribade', 'gay_woman', 'Lesbian', 'sapphic'], ['couples', 'couple', 'twosome', 'duo', 'duet', 'mates', 'match', 'pair', 'twain', 'brace', 'span', 'yoke', 'couplet', 'distich', 'dyad', 'duad', 'mate', 'twin', 'couple_on', 'couple_up', 'pair_off', 'partner_off', 'copulate'], ['platonic', 'Platonic'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk']]</t>
+  </si>
+  <si>
+    <t>[['grandfathers', 'grandfather', 'gramps', 'granddad', 'grandad', 'granddaddy', 'grandpa'], ['caldecott'], ['medal', 'decoration', 'laurel_wreath', 'medallion', 'palm', 'ribbon'], ['voyages', 'ocean_trip', 'voyage', 'sail', 'navigate'], ['travels', 'travel', 'traveling', 'travelling', 'change_of_location', 'locomotion', 'go', 'move', 'locomote', 'journey', 'trip', 'jaunt', 'move_around'], ['homesickness'], ['early', 'former', 'other', 'early_on', 'ahead_of_time', 'too_soon', 'betimes'], ['childhood', 'puerility'], ['instruction', 'direction', 'education', 'teaching', 'pedagogy', 'didactics', 'educational_activity', 'command', 'statement', 'program_line'], ['children', 'child', 'kid', 'youngster', 'minor', 'shaver', 'nipper', 'small_fry', 'tiddler', 'tike', 'tyke', 'fry', 'nestling', 'baby'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['social', 'sociable', 'mixer', 'societal'], ['issues', 'issue', 'number', 'topic', 'subject', 'matter', 'issuing', 'issuance', 'military_issue', 'government_issue', 'return', 'take', 'takings', 'proceeds', 'yield', 'payoff', 'consequence', 'effect', 'outcome', 'result', 'event', 'upshot', 'offspring', 'progeny', 'emergence', 'egress', 'exit', 'outlet', 'way_out', 'publication', 'publish', 'bring_out', 'put_out', 'release', 'supply', 'emerge', 'come_out', 'come_forth', 'go_forth', 'write_out', 'make_out', 'cut'], ['japanese', 'Japanese', 'Nipponese'], ['americans', 'American', 'American_English', 'American_language']]</t>
+  </si>
+  <si>
+    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['poetry', 'poesy', 'verse'], ['french', 'French', 'French_people', 'Daniel_Chester_French', 'Gallic'], ['literature', 'lit'], ['medieval', 'mediaeval', 'gothic', 'chivalric', 'knightly'], ['romances', 'love_affair', 'romance', 'romanticism', 'Romance', 'Romance_language', 'Latinian_language', 'love_story', 'woo', 'court', 'solicit', 'chat_up', 'flirt', 'dally', 'butterfly', 'coquet', 'coquette', 'philander', 'mash'], ['manuscripts', 'manuscript', 'ms', 'holograph'], ['courtly', 'formal', 'stately']]</t>
+  </si>
+  <si>
     <t>[['man', 'adult_male', 'serviceman', 'military_man', 'military_personnel', 'homo', 'human_being', 'human', 'valet', 'valet_de_chambre', 'gentleman', "gentleman's_gentleman", 'Man', 'Isle_of_Man', 'piece', 'world', 'human_race', 'humanity', 'humankind', 'human_beings', 'humans', 'mankind'], ['woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['relationships', 'relationship', 'human_relationship', 'kinship', 'family_relationship'], ['married', 'marry', 'get_married', 'wed', 'conjoin', 'hook_up_with', 'get_hitched_with', 'espouse', 'tie', 'splice', 'marital', 'matrimonial'], ['people', 'citizenry', 'multitude', 'masses', 'mass', 'hoi_polloi', 'the_great_unwashed']]</t>
   </si>
   <si>
+    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['poetry', 'poesy', 'verse'], ['greek', 'Greek', 'Hellenic', 'Hellenic_language', 'Hellene', 'Grecian']]</t>
+  </si>
+  <si>
+    <t>[['sonnets', 'sonnet'], ['english', 'English', 'English_language', 'English_people', 'side'], ['poetry', 'poesy', 'verse'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk']]</t>
+  </si>
+  <si>
+    <t>[['queens', 'Queens', 'queen', 'queen_regnant', 'female_monarch', 'king', 'world-beater', 'fagot', 'faggot', 'fag', 'fairy', 'nance', 'pansy', 'queer', 'poof', 'poove', 'pouf', 'queen_mole_rat', 'tabby'], ['war', 'warfare', 'state_of_war'], ['authors', 'writer', 'author', 'generator', 'source'], ['welsh', 'Welshman', 'Welsh', 'Cambrian', 'Cymry', 'Cymric', 'Welsh_Black', 'welch'], ['soldiers', 'soldier'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['letters', 'letter', 'missive', 'letter_of_the_alphabet', 'alphabetic_character', 'varsity_letter']]</t>
+  </si>
+  <si>
+    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['friendship', 'friendly_relationship']]</t>
+  </si>
+  <si>
     <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk']]</t>
   </si>
   <si>
-    <t>[['queens', 'Queens', 'queen', 'queen_regnant', 'female_monarch', 'king', 'world-beater', 'fagot', 'faggot', 'fag', 'fairy', 'nance', 'pansy', 'queer', 'poof', 'poove', 'pouf', 'queen_mole_rat', 'tabby'], ['war', 'warfare', 'state_of_war'], ['authors', 'writer', 'author', 'generator', 'source'], ['welsh', 'Welshman', 'Welsh', 'Cambrian', 'Cymry', 'Cymric', 'Welsh_Black', 'welch'], ['soldiers', 'soldier'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['letters', 'letter', 'missive', 'letter_of_the_alphabet', 'alphabetic_character', 'varsity_letter']]</t>
-  </si>
-  <si>
-    <t>[['couples', 'couple', 'twosome', 'duo', 'duet', 'mates', 'match', 'pair', 'twain', 'brace', 'span', 'yoke', 'couplet', 'distich', 'dyad', 'duad', 'mate', 'twin', 'couple_on', 'couple_up', 'pair_off', 'partner_off', 'copulate'], ['selection', 'choice', 'option', 'pick', 'survival', 'survival_of_the_fittest', 'natural_selection', 'excerpt', 'excerption', 'extract'], ['man', 'adult_male', 'serviceman', 'military_man', 'military_personnel', 'homo', 'human_being', 'human', 'valet', 'valet_de_chambre', 'gentleman', "gentleman's_gentleman", 'Man', 'Isle_of_Man', 'piece', 'world', 'human_race', 'humanity', 'humankind', 'human_beings', 'humans', 'mankind'], ['woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['relationships', 'relationship', 'human_relationship', 'kinship', 'family_relationship'], ['dating', 'geological_dating', 'date', 'date_stamp', 'go_steady', 'go_out', 'see'], ['social', 'sociable', 'mixer', 'societal'], ['customs', 'customs_duty', 'custom', 'impost', 'usage', 'usance', 'tradition'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk']]</t>
-  </si>
-  <si>
-    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['detective', 'investigator', 'tec', 'police_detective'], ['mystery', 'enigma', 'secret', 'closed_book', 'mystery_story', 'whodunit']]</t>
-  </si>
-  <si>
-    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['english', 'English', 'English_language', 'English_people', 'side'], ['american', 'American', 'American_English', 'American_language'], ['fiction', 'fabrication', 'fable']]</t>
-  </si>
-  <si>
-    <t>[['self', 'ego'], ['actualization', 'realization', 'realisation', 'actualisation'], ['psychology', 'psychological_science'], ['maturation', 'ripening', 'maturement', 'growth', 'growing', 'development', 'ontogeny', 'ontogenesis', 'festering', 'suppuration'], ['interpersonal'], ['relations', 'dealings', 'relation', 'sexual_intercourse', 'intercourse', 'sex_act', 'copulation', 'coitus', 'coition', 'sexual_congress', 'congress', 'sexual_relation', 'carnal_knowledge', 'relative', 'telling', 'recounting', 'relation_back'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['values', 'value', 'economic_value', 'time_value', 'note_value', 'prize', 'treasure', 'appreciate', 'respect', 'esteem', 'prise', 'measure', 'evaluate', 'valuate', 'assess', 'appraise', 'rate'], ['spirituality', 'spiritualty', 'church_property', 'spiritualism', 'spiritism', 'otherworldliness']]</t>
-  </si>
-  <si>
-    <t>[['horror', 'repugnance', 'repulsion', 'revulsion'], ['tales', 'narrative', 'narration', 'story', 'tale', 'fib', 'tarradiddle', 'taradiddle'], ['books', 'book', 'volume', 'record', 'record_book', 'script', 'playscript', 'ledger', 'leger', 'account_book', 'book_of_account', 'rule_book', 'Koran', 'Quran', "al-Qur'an", 'Book', 'Bible', 'Christian_Bible', 'Good_Book', 'Holy_Scripture', 'Holy_Writ', 'Scripture', 'Word_of_God', 'Word', 'reserve', 'hold'], ['reading', 'meter_reading', 'indication', 'reading_material', 'interpretation', 'version', 'Reading', 'recitation', 'recital', 'read', 'say', 'scan', 'take', 'learn', 'study', 'register', 'show', 'record', 'understand', 'interpret', 'translate'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['english', 'English', 'English_language', 'English_people', 'side']]</t>
-  </si>
-  <si>
-    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['american', 'American', 'American_English', 'American_language'], ['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['authors', 'writer', 'author', 'generator', 'source'], ['readers', 'reader', 'subscriber', 'reviewer', 'referee', 'proofreader', 'lector', 'lecturer'], ['sex', 'sexual_activity', 'sexual_practice', 'sex_activity', 'sexual_urge', 'gender', 'sexuality', 'arouse', 'excite', 'turn_on', 'wind_up'], ['role', 'function', 'office', 'part', 'character', 'theatrical_role', 'persona', 'purpose', 'use'], ['literature', 'lit']]</t>
+    <t>[['marriage', 'matrimony', 'union', 'spousal_relationship', 'wedlock', 'married_couple', 'man_and_wife', 'wedding', 'marriage_ceremony'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk']]</t>
   </si>
   <si>
     <t>[['monsters', 'monster', 'giant', 'goliath', 'behemoth', 'colossus', 'freak', 'monstrosity', 'lusus_naturae', 'fiend', 'devil', 'demon', 'ogre', 'teras'], ['baseball', 'baseball_game'], ['early', 'former', 'other', 'early_on', 'ahead_of_time', 'too_soon', 'betimes'], ['childhood', 'puerility'], ['instruction', 'direction', 'education', 'teaching', 'pedagogy', 'didactics', 'educational_activity', 'command', 'statement', 'program_line'], ['children', 'child', 'kid', 'youngster', 'minor', 'shaver', 'nipper', 'small_fry', 'tiddler', 'tike', 'tyke', 'fry', 'nestling', 'baby'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle']]</t>
@@ -523,100 +613,10 @@
     <t>[['wizards', 'ace', 'adept', 'champion', 'sensation', 'maven', 'mavin', 'virtuoso', 'genius', 'hotshot', 'star', 'superstar', 'whiz', 'whizz', 'wizard', 'wiz', 'sorcerer', 'magician', 'necromancer', 'thaumaturge', 'thaumaturgist'], ['magic', 'thaumaturgy', 'magic_trick', 'conjuring_trick', 'trick', 'legerdemain', 'conjuration', 'illusion', 'deception', 'charming', 'magical', 'sorcerous', 'witching', 'wizard', 'wizardly'], ['animals', 'animal', 'animate_being', 'beast', 'brute', 'creature', 'fauna'], ['witchcraft', 'witchery'], ['early', 'former', 'other', 'early_on', 'ahead_of_time', 'too_soon', 'betimes'], ['childhood', 'puerility'], ['instruction', 'direction', 'education', 'teaching', 'pedagogy', 'didactics', 'educational_activity', 'command', 'statement', 'program_line'], ['children', 'child', 'kid', 'youngster', 'minor', 'shaver', 'nipper', 'small_fry', 'tiddler', 'tike', 'tyke', 'fry', 'nestling', 'baby'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle']]</t>
   </si>
   <si>
-    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['soul', 'psyche', 'person', 'individual', 'someone', 'somebody', 'mortal', 'soulfulness'], ['rhetoric', 'grandiosity', 'magniloquence', 'ornateness', 'grandiloquence', 'palaver', 'hot_air', 'empty_words', 'empty_talk'], ['ancient', 'antediluvian']]</t>
-  </si>
-  <si>
-    <t>[['comedy', 'drollery', 'clowning', 'funniness'], ['films', 'movie', 'film', 'picture', 'moving_picture', 'moving-picture_show', 'motion_picture', 'motion-picture_show', 'picture_show', 'pic', 'flick', 'cinema', 'celluloid', 'photographic_film', 'plastic_film', 'shoot', 'take'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['motion', 'gesture', 'movement', 'move', 'motility', 'question', 'apparent_motion', 'apparent_movement', 'gesticulate'], ['pictures', 'picture', 'image', 'icon', 'ikon', 'painting', 'mental_picture', 'impression', 'scene', 'pictorial_matter', 'movie', 'film', 'moving_picture', 'moving-picture_show', 'motion_picture', 'motion-picture_show', 'picture_show', 'pic', 'flick', 'video', 'word_picture', 'word-painting', 'delineation', 'depiction', 'characterization', 'characterisation', 'photograph', 'photo', 'exposure', 'visualize', 'visualise', 'envision', 'project', 'fancy', 'see', 'figure', 'depict', 'render', 'show']]</t>
-  </si>
-  <si>
-    <t>[['english', 'English', 'English_language', 'English_people', 'side'], ['fiction', 'fabrication', 'fable'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['literature', 'lit']]</t>
-  </si>
-  <si>
-    <t>[['literature', 'lit'], ['historical', 'historic', 'diachronic'], ['fiction', 'fabrication', 'fable'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle']]</t>
-  </si>
-  <si>
-    <t>[['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['literature', 'lit'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['english', 'English', 'English_language', 'English_people', 'side']]</t>
-  </si>
-  <si>
-    <t>[['english', 'English', 'English_language', 'English_people', 'side'], ['fiction', 'fabrication', 'fable'], ['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['literature', 'lit'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle']]</t>
-  </si>
-  <si>
-    <t>[['french', 'French', 'French_people', 'Daniel_Chester_French', 'Gallic'], ['fiction', 'fabrication', 'fable'], ['epistolary', 'epistolatory'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['literature', 'lit'], ['letters', 'letter', 'missive', 'letter_of_the_alphabet', 'alphabetic_character', 'varsity_letter']]</t>
-  </si>
-  <si>
-    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['poetry', 'poesy', 'verse'], ['european', 'European'], ['literature', 'lit'], ['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['sex', 'sexual_activity', 'sexual_practice', 'sex_activity', 'sexual_urge', 'gender', 'sexuality', 'arouse', 'excite', 'turn_on', 'wind_up'], ['role', 'function', 'office', 'part', 'character', 'theatrical_role', 'persona', 'purpose', 'use']]</t>
-  </si>
-  <si>
-    <t>[['chastity', 'celibacy', 'sexual_abstention', 'virtue', 'sexual_morality'], ['literature', 'lit'], ['english', 'English', 'English_language', 'English_people', 'side'], ['feminism', 'feminist_movement', "women's_liberation_movement", "women's_lib"], ['kings', 'king', 'male_monarch', 'Rex', 'queen', 'world-beater', 'baron', 'big_businessman', 'business_leader', 'magnate', 'mogul', 'power', 'top_executive', 'tycoon', 'King', 'Billie_Jean_King', 'Billie_Jean_Moffitt_King', 'B._B._King', 'Riley_B_King', 'Martin_Luther_King', 'Martin_Luther_King_Jr.'], ['rulers', 'ruler', 'swayer', 'rule'], ['kings', 'king', 'male_monarch', 'Rex', 'queen', 'world-beater', 'baron', 'big_businessman', 'business_leader', 'magnate', 'mogul', 'power', 'top_executive', 'tycoon', 'King', 'Billie_Jean_King', 'Billie_Jean_Moffitt_King', 'B._B._King', 'Riley_B_King', 'Martin_Luther_King', 'Martin_Luther_King_Jr.'], ['social', 'sociable', 'mixer', 'societal'], ['sciences', 'science', 'scientific_discipline', 'skill'], ['queens', 'Queens', 'queen', 'queen_regnant', 'female_monarch', 'king', 'world-beater', 'fagot', 'faggot', 'fag', 'fairy', 'nance', 'pansy', 'queer', 'poof', 'poove', 'pouf', 'queen_mole_rat', 'tabby'], ['sex', 'sexual_activity', 'sexual_practice', 'sex_activity', 'sexual_urge', 'gender', 'sexuality', 'arouse', 'excite', 'turn_on', 'wind_up'], ['role', 'function', 'office', 'part', 'character', 'theatrical_role', 'persona', 'purpose', 'use'], ['single', 'bingle', 'one', '1', 'I', 'ace', 'unity', 'individual', 'unmarried', 'undivided', 'exclusive'], ['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex']]</t>
-  </si>
-  <si>
-    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['poetry', 'poesy', 'verse'], ['greek', 'Greek', 'Hellenic', 'Hellenic_language', 'Hellene', 'Grecian']]</t>
-  </si>
-  <si>
-    <t>[['lesbian', 'tribade', 'gay_woman', 'Lesbian', 'sapphic'], ['couples', 'couple', 'twosome', 'duo', 'duet', 'mates', 'match', 'pair', 'twain', 'brace', 'span', 'yoke', 'couplet', 'distich', 'dyad', 'duad', 'mate', 'twin', 'couple_on', 'couple_up', 'pair_off', 'partner_off', 'copulate'], ['platonic', 'Platonic'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk']]</t>
-  </si>
-  <si>
-    <t>[['sonnets', 'sonnet'], ['english', 'English', 'English_language', 'English_people', 'side'], ['poetry', 'poesy', 'verse'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk']]</t>
-  </si>
-  <si>
-    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['poetry', 'poesy', 'verse'], ['european', 'European'], ['latin', 'Latin', 'Romance'], ['medieval', 'mediaeval', 'gothic', 'chivalric', 'knightly'], ['modern', 'modern_font', 'Bodoni', 'Bodoni_font', 'mod', 'modernistic', 'advanced', 'forward-looking', 'innovative', 'Modern', 'New']]</t>
-  </si>
-  <si>
-    <t>[['governesses', 'governess', 'regulate', 'regularize', 'regularise', 'order', 'govern', 'rule'], ['fathers', 'father', 'male_parent', 'begetter', 'forefather', 'sire', 'Father', 'Padre', 'Church_Father', 'Father_of_the_Church', 'Father-God', 'Fatherhood', 'founder', 'beginner', 'founding_father', 'don', 'beget', 'get', 'engender', 'mother', 'generate', 'bring_forth'], ['daughters', 'daughter', 'girl'], ['mentally'], ['ill', 'ailment', 'complaint', 'sick', 'inauspicious', 'ominous', 'badly', 'poorly'], ['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['charity', 'brotherly_love', "Jacob's_ladder", 'Greek_valerian', 'Polemonium_caeruleum', 'Polemonium_van-bruntiae', 'Polymonium_caeruleum_van-bruntiae'], ['schools', 'school', 'schoolhouse', 'schooling', 'schooltime', 'school_day', 'shoal', 'educate', 'train', 'cultivate', 'civilize', 'civilise'], ['married', 'marry', 'get_married', 'wed', 'conjoin', 'hook_up_with', 'get_hitched_with', 'espouse', 'tie', 'splice', 'marital', 'matrimonial'], ['people', 'citizenry', 'multitude', 'masses', 'mass', 'hoi_polloi', 'the_great_unwashed'], ['country', 'state', 'nation', 'land', 'commonwealth', 'res_publica', 'body_politic', 'rural_area', 'area'], ['homes', 'home', 'place', 'dwelling', 'domicile', 'abode', 'habitation', 'dwelling_house', 'home_plate', 'home_base', 'plate', 'base', 'family', 'household', 'house', 'menage', 'nursing_home', 'rest_home'], ['youth', 'young_person', 'younker', 'spring_chicken', 'young', 'early_days', 'youthfulness', 'juvenility'], ['orphans', 'orphan']]</t>
-  </si>
-  <si>
-    <t>[['marriage', 'matrimony', 'union', 'spousal_relationship', 'wedlock', 'married_couple', 'man_and_wife', 'wedding', 'marriage_ceremony'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk']]</t>
-  </si>
-  <si>
-    <t>[['poetry', 'poesy', 'verse'], ['satire', 'sarcasm', 'irony', 'caustic_remark'], ['latin', 'Latin', 'Romance'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['poetry', 'poesy', 'verse'], ['epigrams', 'epigram', 'quip']]</t>
-  </si>
-  <si>
-    <t>[['old', 'older', 'erstwhile', 'former', 'onetime', 'one-time', 'quondam', 'sometime', 'honest-to-god', 'honest-to-goodness', 'sure-enough', 'Old', 'previous'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['self', 'ego'], ['values', 'value', 'economic_value', 'time_value', 'note_value', 'prize', 'treasure', 'appreciate', 'respect', 'esteem', 'prise', 'measure', 'evaluate', 'valuate', 'assess', 'appraise', 'rate'], ['large', 'big', 'bombastic', 'declamatory', 'orotund', 'tumid', 'turgid', 'magnanimous', 'prominent', 'enceinte', 'expectant', 'gravid', 'great', 'heavy', 'with_child', 'boastfully', 'vauntingly'], ['characters', 'fictional_character', 'fictitious_character', 'character', 'quality', 'lineament', 'fiber', 'fibre', 'role', 'theatrical_role', 'part', 'persona', 'eccentric', 'type', 'case', 'reference', 'character_reference', 'grapheme', 'graphic_symbol'], ['books', 'book', 'volume', 'record', 'record_book', 'script', 'playscript', 'ledger', 'leger', 'account_book', 'book_of_account', 'rule_book', 'Koran', 'Quran', "al-Qur'an", 'Book', 'Bible', 'Christian_Bible', 'Good_Book', 'Holy_Scripture', 'Holy_Writ', 'Scripture', 'Word_of_God', 'Word', 'reserve', 'hold']]</t>
-  </si>
-  <si>
-    <t>[['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['literature', 'lit'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['french', 'French', 'French_people', 'Daniel_Chester_French', 'Gallic'], ['characters', 'fictional_character', 'fictitious_character', 'character', 'quality', 'lineament', 'fiber', 'fibre', 'role', 'theatrical_role', 'part', 'persona', 'eccentric', 'type', 'case', 'reference', 'character_reference', 'grapheme', 'graphic_symbol'], ['characteristics', 'feature', 'characteristic', 'device_characteristic'], ['narration', 'narrative', 'story', 'tale', 'recital', 'yarn'], ['rhetoric', 'grandiosity', 'magniloquence', 'ornateness', 'grandiloquence', 'palaver', 'hot_air', 'empty_words', 'empty_talk'], ['literary'], ['classes', 'class', 'category', 'family', 'form', 'grade', 'course', 'stratum', 'social_class', 'socio-economic_class', 'course_of_study', 'course_of_instruction', 'division', 'year', 'classify', 'sort', 'assort', 'sort_out', 'separate']]</t>
-  </si>
-  <si>
-    <t>[['erotic', 'titillating'], ['poetry', 'poesy', 'verse'], ['english', 'English', 'English_language', 'English_people', 'side'], ['epic', 'epic_poem', 'heroic_poem', 'epos', 'heroic', 'larger-than-life', 'epical'], ['desire', 'want', 'hope', 'trust'], ['literature', 'lit'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['sex', 'sexual_activity', 'sexual_practice', 'sex_activity', 'sexual_urge', 'gender', 'sexuality', 'arouse', 'excite', 'turn_on', 'wind_up']]</t>
+    <t>[['tlingit', 'Tlingit'], ['indians', 'Indian', 'American_Indian', 'Red_Indian', 'Amerind', 'Amerindian_language', 'American-Indian_language'], ['haida', 'Haida'], ['mythology'], ['ethnic', 'cultural', 'ethnical', 'heathen', 'heathenish', 'pagan'], ['race', 'subspecies', 'slipstream', 'airstream', 'backwash', 'wash', 'raceway', 'rush', 'hotfoot', 'hasten', 'hie', 'speed', 'pelt_along', 'rush_along', 'cannonball_along', 'bucket_along', 'belt_along', 'step_on_it', 'run'], ['studies', 'survey', 'study', 'work', 'report', 'written_report', 'discipline', 'subject', 'subject_area', 'subject_field', 'field', 'field_of_study', 'bailiwick', 'sketch', 'cogitation', 'analyze', 'analyse', 'examine', 'canvass', 'canvas', 'consider', 'learn', 'read', 'take', 'hit_the_books', 'meditate', 'contemplate'], ['sex', 'sexual_activity', 'sexual_practice', 'sex_activity', 'sexual_urge', 'gender', 'sexuality', 'arouse', 'excite', 'turn_on', 'wind_up'], ['social', 'sociable', 'mixer', 'societal'], ['sciences', 'science', 'scientific_discipline', 'skill']]</t>
   </si>
   <si>
     <t>[['aging', 'ripening', 'ageing', 'senescence', 'age', 'senesce', 'get_on', 'mature', 'maturate', 'senescent']]</t>
-  </si>
-  <si>
-    <t>[['sex', 'sexual_activity', 'sexual_practice', 'sex_activity', 'sexual_urge', 'gender', 'sexuality', 'arouse', 'excite', 'turn_on', 'wind_up'], ['christian', 'Christian'], ['life', 'living', 'animation', 'aliveness', 'lifetime', 'life-time', 'lifespan', 'liveliness', 'spirit', 'sprightliness', 'biography', 'life_story', 'life_history', 'life_sentence']]</t>
-  </si>
-  <si>
-    <t>[['english', 'English', 'English_language', 'English_people', 'side'], ['city', 'metropolis', 'urban_center'], ['town', 'townspeople', 'townsfolk', 'township', 'Town', 'Ithiel_Town'], ['life', 'living', 'animation', 'aliveness', 'lifetime', 'life-time', 'lifespan', 'liveliness', 'spirit', 'sprightliness', 'biography', 'life_story', 'life_history', 'life_sentence'], ['married', 'marry', 'get_married', 'wed', 'conjoin', 'hook_up_with', 'get_hitched_with', 'espouse', 'tie', 'splice', 'marital', 'matrimonial'], ['people', 'citizenry', 'multitude', 'masses', 'mass', 'hoi_polloi', 'the_great_unwashed'], ['youth', 'young_person', 'younker', 'spring_chicken', 'young', 'early_days', 'youthfulness', 'juvenility'], ['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex']]</t>
-  </si>
-  <si>
-    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['friendship', 'friendly_relationship']]</t>
-  </si>
-  <si>
-    <t>[['grandfathers', 'grandfather', 'gramps', 'granddad', 'grandad', 'granddaddy', 'grandpa'], ['caldecott'], ['medal', 'decoration', 'laurel_wreath', 'medallion', 'palm', 'ribbon'], ['voyages', 'ocean_trip', 'voyage', 'sail', 'navigate'], ['travels', 'travel', 'traveling', 'travelling', 'change_of_location', 'locomotion', 'go', 'move', 'locomote', 'journey', 'trip', 'jaunt', 'move_around'], ['homesickness'], ['early', 'former', 'other', 'early_on', 'ahead_of_time', 'too_soon', 'betimes'], ['childhood', 'puerility'], ['instruction', 'direction', 'education', 'teaching', 'pedagogy', 'didactics', 'educational_activity', 'command', 'statement', 'program_line'], ['children', 'child', 'kid', 'youngster', 'minor', 'shaver', 'nipper', 'small_fry', 'tiddler', 'tike', 'tyke', 'fry', 'nestling', 'baby'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['social', 'sociable', 'mixer', 'societal'], ['issues', 'issue', 'number', 'topic', 'subject', 'matter', 'issuing', 'issuance', 'military_issue', 'government_issue', 'return', 'take', 'takings', 'proceeds', 'yield', 'payoff', 'consequence', 'effect', 'outcome', 'result', 'event', 'upshot', 'offspring', 'progeny', 'emergence', 'egress', 'exit', 'outlet', 'way_out', 'publication', 'publish', 'bring_out', 'put_out', 'release', 'supply', 'emerge', 'come_out', 'come_forth', 'go_forth', 'write_out', 'make_out', 'cut'], ['japanese', 'Japanese', 'Nipponese'], ['americans', 'American', 'American_English', 'American_language']]</t>
-  </si>
-  <si>
-    <t>[['courtly', 'formal', 'stately'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['literature', 'lit'], ['poetry', 'poesy', 'verse'], ['latin', 'Latin', 'Romance'], ['medieval', 'mediaeval', 'gothic', 'chivalric', 'knightly'], ['modern', 'modern_font', 'Bodoni', 'Bodoni_font', 'mod', 'modernistic', 'advanced', 'forward-looking', 'innovative', 'Modern', 'New']]</t>
-  </si>
-  <si>
-    <t>[['spanish', 'Spanish', 'Spanish_people'], ['poetry', 'poesy', 'verse'], ['courtly', 'formal', 'stately'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['literature', 'lit'], ['authors', 'writer', 'author', 'generator', 'source'], ['patrons', 'patron', 'frequenter', 'sponsor', 'supporter']]</t>
-  </si>
-  <si>
-    <t>[['old', 'older', 'erstwhile', 'former', 'onetime', 'one-time', 'quondam', 'sometime', 'honest-to-god', 'honest-to-goodness', 'sure-enough', 'Old', 'previous'], ['christianity', 'Christianity', 'Christian_religion', 'Christendom'], ['providence', 'Providence', 'capital_of_Rhode_Island'], ['government', 'authorities', 'regime', 'governing', 'governance', 'government_activity', 'administration', 'politics', 'political_science'], ['color', 'colour', 'coloring', 'colouring', 'vividness', 'coloration', 'colouration', 'people_of_color', 'people_of_colour', 'semblance', 'gloss', 'coloring_material', 'colouring_material', 'colorize', 'colorise', 'colourise', 'colourize', 'color_in', 'colour_in', 'tinge', 'distort', 'emblazon', 'discolor', 'discolour'], ['early', 'former', 'other', 'early_on', 'ahead_of_time', 'too_soon', 'betimes'], ['childhood', 'puerility'], ['instruction', 'direction', 'education', 'teaching', 'pedagogy', 'didactics', 'educational_activity', 'command', 'statement', 'program_line'], ['children', 'child', 'kid', 'youngster', 'minor', 'shaver', 'nipper', 'small_fry', 'tiddler', 'tike', 'tyke', 'fry', 'nestling', 'baby'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle']]</t>
-  </si>
-  <si>
-    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['poetry', 'poesy', 'verse'], ['latin', 'Latin', 'Romance'], ['psychoanalysis', 'analysis', 'depth_psychology'], ['literature', 'lit'], ['desire', 'want', 'hope', 'trust'], ['narration', 'narrative', 'story', 'tale', 'recital', 'yarn'], ['rhetoric', 'grandiosity', 'magniloquence', 'ornateness', 'grandiloquence', 'palaver', 'hot_air', 'empty_words', 'empty_talk'], ['rome', 'Rome', 'Roma', 'Eternal_City', 'Italian_capital', 'capital_of_Italy'], ['ancient', 'antediluvian']]</t>
-  </si>
-  <si>
-    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['literature', 'lit'], ['european', 'European'], ['friendship', 'friendly_relationship']]</t>
-  </si>
-  <si>
-    <t>[['man', 'adult_male', 'serviceman', 'military_man', 'military_personnel', 'homo', 'human_being', 'human', 'valet', 'valet_de_chambre', 'gentleman', "gentleman's_gentleman", 'Man', 'Isle_of_Man', 'piece', 'world', 'human_race', 'humanity', 'humankind', 'human_beings', 'humans', 'mankind'], ['woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['relationships', 'relationship', 'human_relationship', 'kinship', 'family_relationship'], ['teenagers', 'adolescent', 'stripling', 'teenager', 'teen'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['couples', 'couple', 'twosome', 'duo', 'duet', 'mates', 'match', 'pair', 'twain', 'brace', 'span', 'yoke', 'couplet', 'distich', 'dyad', 'duad', 'mate', 'twin', 'couple_on', 'couple_up', 'pair_off', 'partner_off', 'copulate'], ['selection', 'choice', 'option', 'pick', 'survival', 'survival_of_the_fittest', 'natural_selection', 'excerpt', 'excerption', 'extract'], ['household', 'family', 'house', 'home', 'menage'], ['marriage', 'matrimony', 'union', 'spousal_relationship', 'wedlock', 'married_couple', 'man_and_wife', 'wedding', 'marriage_ceremony'], ['sociology'], ['social', 'sociable', 'mixer', 'societal'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['sciences', 'science', 'scientific_discipline', 'skill']]</t>
-  </si>
-  <si>
-    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['poetry', 'poesy', 'verse'], ['french', 'French', 'French_people', 'Daniel_Chester_French', 'Gallic'], ['literature', 'lit'], ['medieval', 'mediaeval', 'gothic', 'chivalric', 'knightly'], ['romances', 'love_affair', 'romance', 'romanticism', 'Romance', 'Romance_language', 'Latinian_language', 'love_story', 'woo', 'court', 'solicit', 'chat_up', 'flirt', 'dally', 'butterfly', 'coquet', 'coquette', 'philander', 'mash'], ['manuscripts', 'manuscript', 'ms', 'holograph'], ['courtly', 'formal', 'stately']]</t>
-  </si>
-  <si>
-    <t>[['tlingit', 'Tlingit'], ['indians', 'Indian', 'American_Indian', 'Red_Indian', 'Amerind', 'Amerindian_language', 'American-Indian_language'], ['haida', 'Haida'], ['mythology'], ['ethnic', 'cultural', 'ethnical', 'heathen', 'heathenish', 'pagan'], ['race', 'subspecies', 'slipstream', 'airstream', 'backwash', 'wash', 'raceway', 'rush', 'hotfoot', 'hasten', 'hie', 'speed', 'pelt_along', 'rush_along', 'cannonball_along', 'bucket_along', 'belt_along', 'step_on_it', 'run'], ['studies', 'survey', 'study', 'work', 'report', 'written_report', 'discipline', 'subject', 'subject_area', 'subject_field', 'field', 'field_of_study', 'bailiwick', 'sketch', 'cogitation', 'analyze', 'analyse', 'examine', 'canvass', 'canvas', 'consider', 'learn', 'read', 'take', 'hit_the_books', 'meditate', 'contemplate'], ['sex', 'sexual_activity', 'sexual_practice', 'sex_activity', 'sexual_urge', 'gender', 'sexuality', 'arouse', 'excite', 'turn_on', 'wind_up'], ['social', 'sociable', 'mixer', 'societal'], ['sciences', 'science', 'scientific_discipline', 'skill']]</t>
   </si>
   <si>
     <t>Book ID</t>
@@ -1023,7 +1023,7 @@
   <cols>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="90.7109375" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
     <col min="5" max="5" width="181.7109375" customWidth="1"/>
     <col min="6" max="6" width="1851.7109375" customWidth="1"/>
   </cols>
@@ -1076,7 +1076,7 @@
         <v>58</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0.6240740740740741</v>
       </c>
       <c r="E3" t="s">
         <v>108</v>
@@ -1093,16 +1093,16 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>0.6240740740740741</v>
       </c>
       <c r="E4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1113,16 +1113,16 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0.5818181818181818</v>
       </c>
       <c r="E5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1133,10 +1133,10 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0.5742424242424242</v>
       </c>
       <c r="E6" t="s">
         <v>110</v>
@@ -1153,16 +1153,16 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0.5555555555555555</v>
       </c>
       <c r="E7" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F7" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1173,16 +1173,16 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0.5162652162652163</v>
       </c>
       <c r="E8" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1196,13 +1196,13 @@
         <v>63</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0.512962962962963</v>
       </c>
       <c r="E9" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="F9" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1216,13 +1216,13 @@
         <v>64</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0.512962962962963</v>
       </c>
       <c r="E10" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F10" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1236,13 +1236,13 @@
         <v>65</v>
       </c>
       <c r="D11">
-        <v>0.9</v>
+        <v>0.512962962962963</v>
       </c>
       <c r="E11" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="F11" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1256,13 +1256,13 @@
         <v>66</v>
       </c>
       <c r="D12">
-        <v>0.9</v>
+        <v>0.512962962962963</v>
       </c>
       <c r="E12" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="F12" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1276,13 +1276,13 @@
         <v>67</v>
       </c>
       <c r="D13">
-        <v>0.8636363636363636</v>
+        <v>0.512962962962963</v>
       </c>
       <c r="E13" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F13" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1293,16 +1293,16 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D14">
-        <v>0.8500000000000001</v>
+        <v>0.512962962962963</v>
       </c>
       <c r="E14" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F14" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1313,16 +1313,16 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D15">
-        <v>0.8363636363636364</v>
+        <v>0.5119528619528619</v>
       </c>
       <c r="E15" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F15" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1336,13 +1336,13 @@
         <v>69</v>
       </c>
       <c r="D16">
-        <v>0.8363636363636364</v>
+        <v>0.5018518518518519</v>
       </c>
       <c r="E16" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F16" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1356,13 +1356,13 @@
         <v>70</v>
       </c>
       <c r="D17">
-        <v>0.8</v>
+        <v>0.4990740740740741</v>
       </c>
       <c r="E17" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="F17" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1376,13 +1376,13 @@
         <v>71</v>
       </c>
       <c r="D18">
-        <v>0.8</v>
+        <v>0.4948199948199948</v>
       </c>
       <c r="E18" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F18" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1396,13 +1396,13 @@
         <v>72</v>
       </c>
       <c r="D19">
-        <v>0.8</v>
+        <v>0.4877104377104377</v>
       </c>
       <c r="E19" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F19" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1416,13 +1416,13 @@
         <v>73</v>
       </c>
       <c r="D20">
-        <v>0.8</v>
+        <v>0.4877104377104377</v>
       </c>
       <c r="E20" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F20" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1436,13 +1436,13 @@
         <v>74</v>
       </c>
       <c r="D21">
-        <v>0.8</v>
+        <v>0.4874125874125874</v>
       </c>
       <c r="E21" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F21" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1456,13 +1456,13 @@
         <v>75</v>
       </c>
       <c r="D22">
-        <v>0.8</v>
+        <v>0.4796296296296296</v>
       </c>
       <c r="E22" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F22" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1476,13 +1476,13 @@
         <v>76</v>
       </c>
       <c r="D23">
-        <v>0.7818181818181819</v>
+        <v>0.4781144781144781</v>
       </c>
       <c r="E23" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F23" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1496,13 +1496,13 @@
         <v>77</v>
       </c>
       <c r="D24">
-        <v>0.7818181818181819</v>
+        <v>0.477933177933178</v>
       </c>
       <c r="E24" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F24" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1516,13 +1516,13 @@
         <v>78</v>
       </c>
       <c r="D25">
-        <v>0.7818181818181819</v>
+        <v>0.4716931216931217</v>
       </c>
       <c r="E25" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F25" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1536,13 +1536,13 @@
         <v>79</v>
       </c>
       <c r="D26">
-        <v>0.7818181818181819</v>
+        <v>0.4707070707070707</v>
       </c>
       <c r="E26" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="F26" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1556,13 +1556,13 @@
         <v>80</v>
       </c>
       <c r="D27">
-        <v>0.7818181818181819</v>
+        <v>0.4681818181818182</v>
       </c>
       <c r="E27" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="F27" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1576,13 +1576,13 @@
         <v>81</v>
       </c>
       <c r="D28">
-        <v>0.7727272727272727</v>
+        <v>0.4681818181818182</v>
       </c>
       <c r="E28" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F28" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1593,16 +1593,16 @@
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D29">
-        <v>0.7727272727272727</v>
+        <v>0.4681818181818182</v>
       </c>
       <c r="E29" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F29" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1613,16 +1613,16 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D30">
-        <v>0.7727272727272727</v>
+        <v>0.4671587671587671</v>
       </c>
       <c r="E30" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F30" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1636,13 +1636,13 @@
         <v>83</v>
       </c>
       <c r="D31">
-        <v>0.7727272727272727</v>
+        <v>0.4656565656565657</v>
       </c>
       <c r="E31" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F31" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1653,16 +1653,16 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D32">
-        <v>0.7727272727272727</v>
+        <v>0.4656565656565657</v>
       </c>
       <c r="E32" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F32" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1676,13 +1676,13 @@
         <v>84</v>
       </c>
       <c r="D33">
-        <v>0.7727272727272727</v>
+        <v>0.4631313131313131</v>
       </c>
       <c r="E33" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="F33" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1696,13 +1696,13 @@
         <v>85</v>
       </c>
       <c r="D34">
-        <v>0.7727272727272727</v>
+        <v>0.462962962962963</v>
       </c>
       <c r="E34" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F34" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1716,13 +1716,13 @@
         <v>86</v>
       </c>
       <c r="D35">
-        <v>0.7727272727272727</v>
+        <v>0.4568181818181818</v>
       </c>
       <c r="E35" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F35" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1736,13 +1736,13 @@
         <v>87</v>
       </c>
       <c r="D36">
-        <v>0.7666666666666666</v>
+        <v>0.4527972027972029</v>
       </c>
       <c r="E36" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F36" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1756,13 +1756,13 @@
         <v>88</v>
       </c>
       <c r="D37">
-        <v>0.7666666666666666</v>
+        <v>0.452020202020202</v>
       </c>
       <c r="E37" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="F37" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1773,16 +1773,16 @@
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D38">
-        <v>0.7575757575757575</v>
+        <v>0.452020202020202</v>
       </c>
       <c r="E38" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F38" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1796,13 +1796,13 @@
         <v>89</v>
       </c>
       <c r="D39">
-        <v>0.7575757575757575</v>
+        <v>0.4478174603174603</v>
       </c>
       <c r="E39" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="F39" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1816,13 +1816,13 @@
         <v>90</v>
       </c>
       <c r="D40">
-        <v>0.7535353535353536</v>
+        <v>0.442929292929293</v>
       </c>
       <c r="E40" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="F40" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1833,16 +1833,16 @@
         <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D41">
-        <v>0.7363636363636363</v>
+        <v>0.442929292929293</v>
       </c>
       <c r="E41" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F41" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1856,13 +1856,13 @@
         <v>91</v>
       </c>
       <c r="D42">
-        <v>0.7363636363636363</v>
+        <v>0.436026936026936</v>
       </c>
       <c r="E42" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F42" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1876,13 +1876,13 @@
         <v>92</v>
       </c>
       <c r="D43">
-        <v>0.7342657342657342</v>
+        <v>0.4353535353535354</v>
       </c>
       <c r="E43" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="F43" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1893,16 +1893,16 @@
         <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D44">
-        <v>0.7272727272727273</v>
+        <v>0.4353535353535354</v>
       </c>
       <c r="E44" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F44" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1913,16 +1913,16 @@
         <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D45">
-        <v>0.7202797202797203</v>
+        <v>0.4353535353535354</v>
       </c>
       <c r="E45" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F45" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1933,16 +1933,16 @@
         <v>44</v>
       </c>
       <c r="C46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D46">
-        <v>0.7202797202797203</v>
+        <v>0.4217171717171717</v>
       </c>
       <c r="E46" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F46" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1953,10 +1953,10 @@
         <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D47">
-        <v>0.7202797202797203</v>
+        <v>0.4217171717171717</v>
       </c>
       <c r="E47" t="s">
         <v>144</v>
@@ -1973,10 +1973,10 @@
         <v>46</v>
       </c>
       <c r="C48" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D48">
-        <v>0.7125</v>
+        <v>0.4126262626262626</v>
       </c>
       <c r="E48" t="s">
         <v>145</v>
@@ -1993,10 +1993,10 @@
         <v>47</v>
       </c>
       <c r="C49" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D49">
-        <v>0.6969696969696969</v>
+        <v>0.3918026418026417</v>
       </c>
       <c r="E49" t="s">
         <v>146</v>
@@ -2013,16 +2013,16 @@
         <v>48</v>
       </c>
       <c r="C50" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D50">
-        <v>0.6969696969696969</v>
+        <v>0.3918026418026417</v>
       </c>
       <c r="E50" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F50" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2036,7 +2036,7 @@
         <v>98</v>
       </c>
       <c r="D51">
-        <v>0.6969696969696969</v>
+        <v>0.3918026418026417</v>
       </c>
       <c r="E51" t="s">
         <v>146</v>
@@ -2053,16 +2053,16 @@
         <v>50</v>
       </c>
       <c r="C52" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D52">
-        <v>0.6909090909090909</v>
+        <v>0.3918026418026417</v>
       </c>
       <c r="E52" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F52" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2073,16 +2073,16 @@
         <v>51</v>
       </c>
       <c r="C53" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D53">
-        <v>0.6865134865134864</v>
+        <v>0.3851851851851851</v>
       </c>
       <c r="E53" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F53" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2093,16 +2093,16 @@
         <v>52</v>
       </c>
       <c r="C54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D54">
-        <v>0.6765734265734266</v>
+        <v>0.3851851851851851</v>
       </c>
       <c r="E54" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F54" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2113,16 +2113,16 @@
         <v>53</v>
       </c>
       <c r="C55" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D55">
-        <v>0.656060606060606</v>
+        <v>0.3851851851851851</v>
       </c>
       <c r="E55" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F55" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2133,16 +2133,16 @@
         <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D56">
-        <v>0.6328671328671328</v>
+        <v>0.3851851851851851</v>
       </c>
       <c r="E56" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F56" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -2156,7 +2156,7 @@
         <v>104</v>
       </c>
       <c r="D57">
-        <v>0.6328671328671328</v>
+        <v>0.3606060606060606</v>
       </c>
       <c r="E57" t="s">
         <v>152</v>
@@ -2176,7 +2176,7 @@
         <v>105</v>
       </c>
       <c r="D58">
-        <v>0.606060606060606</v>
+        <v>0.2526936026936027</v>
       </c>
       <c r="E58" t="s">
         <v>153</v>

</xml_diff>

<commit_message>
move files ans create model
</commit_message>
<xml_diff>
--- a/BackEnd/files/report.xlsx
+++ b/BackEnd/files/report.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="198">
   <si>
     <t>991000001799704574</t>
   </si>
@@ -22,15 +22,9 @@
     <t>991000364949704574</t>
   </si>
   <si>
-    <t>991000050149704574</t>
-  </si>
-  <si>
     <t>991000220919704574</t>
   </si>
   <si>
-    <t>991000027049704574</t>
-  </si>
-  <si>
     <t>991000254419704574</t>
   </si>
   <si>
@@ -49,12 +43,12 @@
     <t>991000072849704574</t>
   </si>
   <si>
+    <t>991000050239704574</t>
+  </si>
+  <si>
     <t>991000365019704574</t>
   </si>
   <si>
-    <t>991000050239704574</t>
-  </si>
-  <si>
     <t>991000236569704574</t>
   </si>
   <si>
@@ -67,12 +61,12 @@
     <t>991000601979704574</t>
   </si>
   <si>
+    <t>991000661829704574</t>
+  </si>
+  <si>
     <t>991000244649704574</t>
   </si>
   <si>
-    <t>991000661829704574</t>
-  </si>
-  <si>
     <t>991000252139704574</t>
   </si>
   <si>
@@ -103,12 +97,12 @@
     <t>991000247059704574</t>
   </si>
   <si>
+    <t>991000067479704574</t>
+  </si>
+  <si>
     <t>991000350969704574</t>
   </si>
   <si>
-    <t>991000067479704574</t>
-  </si>
-  <si>
     <t>991000157529704574</t>
   </si>
   <si>
@@ -148,24 +142,24 @@
     <t>991000107239704574</t>
   </si>
   <si>
+    <t>991000399779704574</t>
+  </si>
+  <si>
     <t>991000080409704574</t>
   </si>
   <si>
-    <t>991000399779704574</t>
-  </si>
-  <si>
     <t>991000070059704574</t>
   </si>
   <si>
+    <t>991000451399704574</t>
+  </si>
+  <si>
+    <t>991000249599704574</t>
+  </si>
+  <si>
     <t>991000252329704574</t>
   </si>
   <si>
-    <t>991000451399704574</t>
-  </si>
-  <si>
-    <t>991000249599704574</t>
-  </si>
-  <si>
     <t>991000244239704574</t>
   </si>
   <si>
@@ -184,9 +178,6 @@
     <t>991001069871904574</t>
   </si>
   <si>
-    <t>991001094844904574</t>
-  </si>
-  <si>
     <t xml:space="preserve">Love and sex after 60 </t>
   </si>
   <si>
@@ -196,9 +187,6 @@
     <t>Transforming desire</t>
   </si>
   <si>
-    <t>The currency of Eros</t>
-  </si>
-  <si>
     <t xml:space="preserve">Sex, dating, and love </t>
   </si>
   <si>
@@ -232,12 +220,12 @@
     <t xml:space="preserve">Middlemarch </t>
   </si>
   <si>
+    <t>Four complete novels /</t>
+  </si>
+  <si>
     <t xml:space="preserve">Erotic faith </t>
   </si>
   <si>
-    <t>Four complete novels /</t>
-  </si>
-  <si>
     <t xml:space="preserve">Free to love again </t>
   </si>
   <si>
@@ -304,15 +292,15 @@
     <t>Love and friendship in Plato and Aristotle</t>
   </si>
   <si>
+    <t>The art of loving</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creating love </t>
+  </si>
+  <si>
     <t xml:space="preserve">The pursuit of love </t>
   </si>
   <si>
-    <t>The art of loving</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Creating love </t>
-  </si>
-  <si>
     <t xml:space="preserve">Getting the love you want </t>
   </si>
   <si>
@@ -331,9 +319,6 @@
     <t xml:space="preserve">Shamans and kushtakas </t>
   </si>
   <si>
-    <t xml:space="preserve">The diary of a man of fifty </t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -346,9 +331,6 @@
     <t>['erotic', 'poetry', 'english', 'epic', 'desire', 'literature', 'love', 'sex']</t>
   </si>
   <si>
-    <t>['love', 'poetry', 'european', 'literature', 'women', 'sex', 'role']</t>
-  </si>
-  <si>
     <t>['dating', 'social', 'customs', 'love', 'sex']</t>
   </si>
   <si>
@@ -382,12 +364,12 @@
     <t>['english', 'city', 'town', 'life', 'married', 'people', 'young', 'women']</t>
   </si>
   <si>
+    <t>['literature', 'historical', 'fiction', 'love', 'stories']</t>
+  </si>
+  <si>
     <t>['english', 'fiction', 'love', 'stories', 'literature']</t>
   </si>
   <si>
-    <t>['literature', 'historical', 'fiction', 'love', 'stories']</t>
-  </si>
-  <si>
     <t>['sex', 'christian', 'life']</t>
   </si>
   <si>
@@ -475,10 +457,7 @@
     <t>['tlingit', 'indians', 'haida', 'mythology', 'ethnic', 'race', 'studies', 'gender', 'social', 'sciences']</t>
   </si>
   <si>
-    <t>['aging']</t>
-  </si>
-  <si>
-    <t>['dXHAyncBufXmZs9o45Vl', 'dnHAyncBufXmZs9o45Vt', 'enHAyncBufXmZs9o45WS', 'eHHAyncBufXmZs9o45WA', 'eXHAyncBufXmZs9o45WJ', 'enHAyncBufXmZs9o45WS', 'b3HAyncBufXmZs9o45Ux']</t>
+    <t>['XENGu3gBqyfetXzjbB2E', 'XUNGu3gBqyfetXzjbB2T', 'XkNGu3gBqyfetXzjbB2p', 'X0NGu3gBqyfetXzjbB29', 'YENGu3gBqyfetXzjbB3O', 'YUNGu3gBqyfetXzjbB3e', 'YkNGu3gBqyfetXzjbB3v']</t>
   </si>
   <si>
     <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['american', 'American', 'American_English', 'American_language'], ['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['authors', 'writer', 'author', 'generator', 'source'], ['readers', 'reader', 'subscriber', 'reviewer', 'referee', 'proofreader', 'lector', 'lecturer'], ['sex', 'sexual_activity', 'sexual_practice', 'sex_activity', 'sexual_urge', 'gender', 'sexuality', 'arouse', 'excite', 'turn_on', 'wind_up'], ['role', 'function', 'office', 'part', 'character', 'theatrical_role', 'persona', 'purpose', 'use'], ['literature', 'lit']]</t>
@@ -487,13 +466,10 @@
     <t>[['erotic', 'titillating'], ['poetry', 'poesy', 'verse'], ['english', 'English', 'English_language', 'English_people', 'side'], ['epic', 'epic_poem', 'heroic_poem', 'epos', 'heroic', 'larger-than-life', 'epical'], ['desire', 'want', 'hope', 'trust'], ['literature', 'lit'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['sex', 'sexual_activity', 'sexual_practice', 'sex_activity', 'sexual_urge', 'gender', 'sexuality', 'arouse', 'excite', 'turn_on', 'wind_up']]</t>
   </si>
   <si>
-    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['poetry', 'poesy', 'verse'], ['european', 'European'], ['literature', 'lit'], ['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['sex', 'sexual_activity', 'sexual_practice', 'sex_activity', 'sexual_urge', 'gender', 'sexuality', 'arouse', 'excite', 'turn_on', 'wind_up'], ['role', 'function', 'office', 'part', 'character', 'theatrical_role', 'persona', 'purpose', 'use']]</t>
-  </si>
-  <si>
     <t>[['dating', 'geological_dating', 'date', 'date_stamp', 'go_steady', 'go_out', 'see'], ['social', 'sociable', 'mixer', 'societal'], ['customs', 'customs_duty', 'custom', 'impost', 'usage', 'usance', 'tradition'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['sex', 'sexual_activity', 'sexual_practice', 'sex_activity', 'sexual_urge', 'gender', 'sexuality', 'arouse', 'excite', 'turn_on', 'wind_up']]</t>
   </si>
   <si>
-    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['poetry', 'poesy', 'verse'], ['latin', 'Latin', 'Romance'], ['psychoanalysis', 'analysis', 'depth_psychology'], ['literature', 'lit'], ['desire', 'want', 'hope', 'trust'], ['narration', 'narrative', 'story', 'tale', 'recital', 'yarn'], ['rhetoric', 'grandiosity', 'magniloquence', 'ornateness', 'grandiloquence', 'palaver', 'hot_air', 'empty_words', 'empty_talk'], ['rome', 'Rome', 'Roma', 'Eternal_City', 'Italian_capital', 'capital_of_Italy'], ['ancient', 'antediluvian']]</t>
+    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['poetry', 'poesy', 'verse'], ['romance', 'love_affair', 'romanticism', 'Romance', 'Romance_language', 'Latinian_language', 'love_story', 'woo', 'court', 'solicit', 'chat_up', 'flirt', 'dally', 'butterfly', 'coquet', 'coquette', 'philander', 'mash', 'Latin'], ['psychoanalysis', 'analysis', 'depth_psychology'], ['literature', 'lit'], ['desire', 'want', 'hope', 'trust'], ['tales', 'narrative', 'narration', 'story', 'tale', 'fib', 'tarradiddle', 'taradiddle'], ['rhetoric', 'grandiosity', 'magniloquence', 'ornateness', 'grandiloquence', 'palaver', 'hot_air', 'empty_words', 'empty_talk'], ['rome', 'Rome', 'Roma', 'Eternal_City', 'Italian_capital', 'capital_of_Italy'], ['ancient', 'antediluvian']]</t>
   </si>
   <si>
     <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['english', 'English', 'English_language', 'English_people', 'side'], ['american', 'American', 'American_English', 'American_language'], ['fiction', 'fabrication', 'fable']]</t>
@@ -508,7 +484,10 @@
     <t>[['french', 'French', 'French_people', 'Daniel_Chester_French', 'Gallic'], ['fiction', 'fabrication', 'fable'], ['epistolary', 'epistolatory'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['literature', 'lit'], ['letters', 'letter', 'missive', 'letter_of_the_alphabet', 'alphabetic_character', 'varsity_letter']]</t>
   </si>
   <si>
-    <t>[['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['literature', 'lit'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['french', 'French', 'French_people', 'Daniel_Chester_French', 'Gallic'], ['characters', 'fictional_character', 'fictitious_character', 'character', 'quality', 'lineament', 'fiber', 'fibre', 'role', 'theatrical_role', 'part', 'persona', 'eccentric', 'type', 'case', 'reference', 'character_reference', 'grapheme', 'graphic_symbol'], ['characteristics', 'feature', 'characteristic', 'device_characteristic'], ['narration', 'narrative', 'story', 'tale', 'recital', 'yarn'], ['rhetoric', 'grandiosity', 'magniloquence', 'ornateness', 'grandiloquence', 'palaver', 'hot_air', 'empty_words', 'empty_talk'], ['literary'], ['classes', 'class', 'category', 'family', 'form', 'grade', 'course', 'stratum', 'social_class', 'socio-economic_class', 'course_of_study', 'course_of_instruction', 'division', 'year', 'classify', 'sort', 'assort', 'sort_out', 'separate']]</t>
+    <t>[['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['literature', 'lit'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['french', 'French', 'French_people', 'Daniel_Chester_French', 'Gallic'], ['characters', 'fictional_character', 'fictitious_character', 'character', 'quality', 'lineament', 'fiber', 'fibre', 'role', 'theatrical_role', 'part', 'persona', 'eccentric', 'type', 'case', 'reference', 'character_reference', 'grapheme', 'graphic_symbol'], ['characteristics', 'feature', 'characteristic', 'device_characteristic'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['rhetoric', 'grandiosity', 'magniloquence', 'ornateness', 'grandiloquence', 'palaver', 'hot_air', 'empty_words', 'empty_talk'], ['literary'], ['classes', 'class', 'category', 'family', 'form', 'grade', 'course', 'stratum', 'social_class', 'socio-economic_class', 'course_of_study', 'course_of_instruction', 'division', 'year', 'classify', 'sort', 'assort', 'sort_out', 'separate']]</t>
+  </si>
+  <si>
+    <t>[['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['literature', 'lit'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['french', 'French', 'French_people', 'Daniel_Chester_French', 'Gallic'], ['characters', 'fictional_character', 'fictitious_character', 'character', 'quality', 'lineament', 'fiber', 'fibre', 'role', 'theatrical_role', 'part', 'persona', 'eccentric', 'type', 'case', 'reference', 'character_reference', 'grapheme', 'graphic_symbol'], ['characteristics', 'feature', 'characteristic', 'device_characteristic'], ['tales', 'narrative', 'narration', 'story', 'tale', 'fib', 'tarradiddle', 'taradiddle'], ['rhetoric', 'grandiosity', 'magniloquence', 'ornateness', 'grandiloquence', 'palaver', 'hot_air', 'empty_words', 'empty_talk'], ['literary'], ['classes', 'class', 'category', 'family', 'form', 'grade', 'course', 'stratum', 'social_class', 'socio-economic_class', 'course_of_study', 'course_of_instruction', 'division', 'year', 'classify', 'sort', 'assort', 'sort_out', 'separate']]</t>
   </si>
   <si>
     <t>[['self', 'ego'], ['actualization', 'realization', 'realisation', 'actualisation'], ['psychology', 'psychological_science'], ['maturation', 'ripening', 'maturement', 'growth', 'growing', 'development', 'ontogeny', 'ontogenesis', 'festering', 'suppuration'], ['interpersonal'], ['relations', 'dealings', 'relation', 'sexual_intercourse', 'intercourse', 'sex_act', 'copulation', 'coitus', 'coition', 'sexual_congress', 'congress', 'sexual_relation', 'carnal_knowledge', 'relative', 'telling', 'recounting', 'relation_back'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['values', 'value', 'economic_value', 'time_value', 'note_value', 'prize', 'treasure', 'appreciate', 'respect', 'esteem', 'prise', 'measure', 'evaluate', 'valuate', 'assess', 'appraise', 'rate'], ['spirituality', 'spiritualty', 'church_property', 'spiritualism', 'spiritism', 'otherworldliness']]</t>
@@ -523,12 +502,12 @@
     <t>[['english', 'English', 'English_language', 'English_people', 'side'], ['city', 'metropolis', 'urban_center'], ['town', 'townspeople', 'townsfolk', 'township', 'Town', 'Ithiel_Town'], ['life', 'living', 'animation', 'aliveness', 'lifetime', 'life-time', 'lifespan', 'liveliness', 'spirit', 'sprightliness', 'biography', 'life_story', 'life_history', 'life_sentence'], ['married', 'marry', 'get_married', 'wed', 'conjoin', 'hook_up_with', 'get_hitched_with', 'espouse', 'tie', 'splice', 'marital', 'matrimonial'], ['people', 'citizenry', 'multitude', 'masses', 'mass', 'hoi_polloi', 'the_great_unwashed'], ['youth', 'young_person', 'younker', 'spring_chicken', 'young', 'early_days', 'youthfulness', 'juvenility'], ['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex']]</t>
   </si>
   <si>
+    <t>[['literature', 'lit'], ['historical', 'historic', 'diachronic'], ['fiction', 'fabrication', 'fable'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle']]</t>
+  </si>
+  <si>
     <t>[['english', 'English', 'English_language', 'English_people', 'side'], ['fiction', 'fabrication', 'fable'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['literature', 'lit']]</t>
   </si>
   <si>
-    <t>[['literature', 'lit'], ['historical', 'historic', 'diachronic'], ['fiction', 'fabrication', 'fable'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle']]</t>
-  </si>
-  <si>
     <t>[['sex', 'sexual_activity', 'sexual_practice', 'sex_activity', 'sexual_urge', 'gender', 'sexuality', 'arouse', 'excite', 'turn_on', 'wind_up'], ['christian', 'Christian'], ['life', 'living', 'animation', 'aliveness', 'lifetime', 'life-time', 'lifespan', 'liveliness', 'spirit', 'sprightliness', 'biography', 'life_story', 'life_history', 'life_sentence']]</t>
   </si>
   <si>
@@ -547,16 +526,16 @@
     <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['literature', 'lit'], ['european', 'European'], ['friendship', 'friendly_relationship']]</t>
   </si>
   <si>
-    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['poetry', 'poesy', 'verse'], ['european', 'European'], ['latin', 'Latin', 'Romance'], ['medieval', 'mediaeval', 'gothic', 'chivalric', 'knightly'], ['modern', 'modern_font', 'Bodoni', 'Bodoni_font', 'mod', 'modernistic', 'advanced', 'forward-looking', 'innovative', 'Modern', 'New']]</t>
-  </si>
-  <si>
-    <t>[['courtly', 'formal', 'stately'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['literature', 'lit'], ['poetry', 'poesy', 'verse'], ['latin', 'Latin', 'Romance'], ['medieval', 'mediaeval', 'gothic', 'chivalric', 'knightly'], ['modern', 'modern_font', 'Bodoni', 'Bodoni_font', 'mod', 'modernistic', 'advanced', 'forward-looking', 'innovative', 'Modern', 'New']]</t>
+    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['poetry', 'poesy', 'verse'], ['european', 'European'], ['romance', 'love_affair', 'romanticism', 'Romance', 'Romance_language', 'Latinian_language', 'love_story', 'woo', 'court', 'solicit', 'chat_up', 'flirt', 'dally', 'butterfly', 'coquet', 'coquette', 'philander', 'mash', 'Latin'], ['medieval', 'mediaeval', 'gothic', 'chivalric', 'knightly'], ['modern', 'modern_font', 'Bodoni', 'Bodoni_font', 'mod', 'modernistic', 'advanced', 'forward-looking', 'innovative', 'Modern', 'New']]</t>
+  </si>
+  <si>
+    <t>[['courtly', 'formal', 'stately'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['literature', 'lit'], ['poetry', 'poesy', 'verse'], ['romance', 'love_affair', 'romanticism', 'Romance', 'Romance_language', 'Latinian_language', 'love_story', 'woo', 'court', 'solicit', 'chat_up', 'flirt', 'dally', 'butterfly', 'coquet', 'coquette', 'philander', 'mash', 'Latin'], ['medieval', 'mediaeval', 'gothic', 'chivalric', 'knightly'], ['modern', 'modern_font', 'Bodoni', 'Bodoni_font', 'mod', 'modernistic', 'advanced', 'forward-looking', 'innovative', 'Modern', 'New']]</t>
   </si>
   <si>
     <t>[['governesses', 'governess', 'regulate', 'regularize', 'regularise', 'order', 'govern', 'rule'], ['fathers', 'father', 'male_parent', 'begetter', 'forefather', 'sire', 'Father', 'Padre', 'Church_Father', 'Father_of_the_Church', 'Father-God', 'Fatherhood', 'founder', 'beginner', 'founding_father', 'don', 'beget', 'get', 'engender', 'mother', 'generate', 'bring_forth'], ['daughters', 'daughter', 'girl'], ['mentally'], ['ill', 'ailment', 'complaint', 'sick', 'inauspicious', 'ominous', 'badly', 'poorly'], ['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['charity', 'brotherly_love', "Jacob's_ladder", 'Greek_valerian', 'Polemonium_caeruleum', 'Polemonium_van-bruntiae', 'Polymonium_caeruleum_van-bruntiae'], ['schools', 'school', 'schoolhouse', 'schooling', 'schooltime', 'school_day', 'shoal', 'educate', 'train', 'cultivate', 'civilize', 'civilise'], ['married', 'marry', 'get_married', 'wed', 'conjoin', 'hook_up_with', 'get_hitched_with', 'espouse', 'tie', 'splice', 'marital', 'matrimonial'], ['people', 'citizenry', 'multitude', 'masses', 'mass', 'hoi_polloi', 'the_great_unwashed'], ['country', 'state', 'nation', 'land', 'commonwealth', 'res_publica', 'body_politic', 'rural_area', 'area'], ['homes', 'home', 'place', 'dwelling', 'domicile', 'abode', 'habitation', 'dwelling_house', 'home_plate', 'home_base', 'plate', 'base', 'family', 'household', 'house', 'menage', 'nursing_home', 'rest_home'], ['youth', 'young_person', 'younker', 'spring_chicken', 'young', 'early_days', 'youthfulness', 'juvenility'], ['orphans', 'orphan']]</t>
   </si>
   <si>
-    <t>[['poetry', 'poesy', 'verse'], ['satire', 'sarcasm', 'irony', 'caustic_remark'], ['latin', 'Latin', 'Romance'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['poetry', 'poesy', 'verse'], ['epigrams', 'epigram', 'quip']]</t>
+    <t>[['poetry', 'poesy', 'verse'], ['satire', 'sarcasm', 'irony', 'caustic_remark'], ['romance', 'love_affair', 'romanticism', 'Romance', 'Romance_language', 'Latinian_language', 'love_story', 'woo', 'court', 'solicit', 'chat_up', 'flirt', 'dally', 'butterfly', 'coquet', 'coquette', 'philander', 'mash', 'Latin'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['poetry', 'poesy', 'verse'], ['epigrams', 'epigram', 'quip']]</t>
   </si>
   <si>
     <t>[['spanish', 'Spanish', 'Spanish_people'], ['poetry', 'poesy', 'verse'], ['courtly', 'formal', 'stately'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['literature', 'lit'], ['authors', 'writer', 'author', 'generator', 'source'], ['patrons', 'patron', 'frequenter', 'sponsor', 'supporter']]</t>
@@ -589,7 +568,7 @@
     <t>[['sonnets', 'sonnet'], ['english', 'English', 'English_language', 'English_people', 'side'], ['poetry', 'poesy', 'verse'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk']]</t>
   </si>
   <si>
-    <t>[['queens', 'Queens', 'queen', 'queen_regnant', 'female_monarch', 'king', 'world-beater', 'fagot', 'faggot', 'fag', 'fairy', 'nance', 'pansy', 'queer', 'poof', 'poove', 'pouf', 'queen_mole_rat', 'tabby'], ['war', 'warfare', 'state_of_war'], ['authors', 'writer', 'author', 'generator', 'source'], ['welsh', 'Welshman', 'Welsh', 'Cambrian', 'Cymry', 'Cymric', 'Welsh_Black', 'welch'], ['soldiers', 'soldier'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['letters', 'letter', 'missive', 'letter_of_the_alphabet', 'alphabetic_character', 'varsity_letter']]</t>
+    <t>[['man', 'adult_male', 'serviceman', 'military_man', 'military_personnel', 'homo', 'human_being', 'human', 'valet', 'valet_de_chambre', 'gentleman', "gentleman's_gentleman", 'Man', 'Isle_of_Man', 'piece', 'world', 'human_race', 'humanity', 'humankind', 'human_beings', 'humans', 'mankind'], ['war', 'warfare', 'state_of_war'], ['authors', 'writer', 'author', 'generator', 'source'], ['welsh', 'Welshman', 'Welsh', 'Cambrian', 'Cymry', 'Cymric', 'Welsh_Black', 'welch'], ['soldiers', 'soldier'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['letters', 'letter', 'missive', 'letter_of_the_alphabet', 'alphabetic_character', 'varsity_letter']]</t>
   </si>
   <si>
     <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['friendship', 'friendly_relationship']]</t>
@@ -614,9 +593,6 @@
   </si>
   <si>
     <t>[['tlingit', 'Tlingit'], ['indians', 'Indian', 'American_Indian', 'Red_Indian', 'Amerind', 'Amerindian_language', 'American-Indian_language'], ['haida', 'Haida'], ['mythology'], ['ethnic', 'cultural', 'ethnical', 'heathen', 'heathenish', 'pagan'], ['race', 'subspecies', 'slipstream', 'airstream', 'backwash', 'wash', 'raceway', 'rush', 'hotfoot', 'hasten', 'hie', 'speed', 'pelt_along', 'rush_along', 'cannonball_along', 'bucket_along', 'belt_along', 'step_on_it', 'run'], ['studies', 'survey', 'study', 'work', 'report', 'written_report', 'discipline', 'subject', 'subject_area', 'subject_field', 'field', 'field_of_study', 'bailiwick', 'sketch', 'cogitation', 'analyze', 'analyse', 'examine', 'canvass', 'canvas', 'consider', 'learn', 'read', 'take', 'hit_the_books', 'meditate', 'contemplate'], ['sex', 'sexual_activity', 'sexual_practice', 'sex_activity', 'sexual_urge', 'gender', 'sexuality', 'arouse', 'excite', 'turn_on', 'wind_up'], ['social', 'sociable', 'mixer', 'societal'], ['sciences', 'science', 'scientific_discipline', 'skill']]</t>
-  </si>
-  <si>
-    <t>[['aging', 'ripening', 'ageing', 'senescence', 'age', 'senesce', 'get_on', 'mature', 'maturate', 'senescent']]</t>
   </si>
   <si>
     <t>Book ID</t>
@@ -1015,7 +991,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F58"/>
+  <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1030,19 +1006,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1">
@@ -1053,16 +1029,16 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1073,16 +1049,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D3">
         <v>0.6240740740740741</v>
       </c>
       <c r="E3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F3" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1093,16 +1069,16 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D4">
-        <v>0.6240740740740741</v>
+        <v>0.5818181818181818</v>
       </c>
       <c r="E4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F4" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1113,16 +1089,16 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D5">
-        <v>0.5818181818181818</v>
+        <v>0.5555555555555555</v>
       </c>
       <c r="E5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="F5" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1133,16 +1109,16 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D6">
-        <v>0.5742424242424242</v>
+        <v>0.5162652162652163</v>
       </c>
       <c r="E6" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F6" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1153,16 +1129,16 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D7">
-        <v>0.5555555555555555</v>
+        <v>0.512962962962963</v>
       </c>
       <c r="E7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F7" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1173,16 +1149,16 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D8">
-        <v>0.5162652162652163</v>
+        <v>0.512962962962963</v>
       </c>
       <c r="E8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F8" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1193,16 +1169,16 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D9">
         <v>0.512962962962963</v>
       </c>
       <c r="E9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="F9" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1213,16 +1189,16 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D10">
         <v>0.512962962962963</v>
       </c>
       <c r="E10" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F10" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1233,16 +1209,16 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D11">
         <v>0.512962962962963</v>
       </c>
       <c r="E11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F11" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1253,16 +1229,16 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D12">
         <v>0.512962962962963</v>
       </c>
       <c r="E12" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F12" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1273,16 +1249,16 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D13">
-        <v>0.512962962962963</v>
+        <v>0.5119528619528619</v>
       </c>
       <c r="E13" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F13" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1293,16 +1269,16 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D14">
-        <v>0.512962962962963</v>
+        <v>0.5018518518518519</v>
       </c>
       <c r="E14" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="F14" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1313,16 +1289,16 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D15">
-        <v>0.5119528619528619</v>
+        <v>0.4990740740740741</v>
       </c>
       <c r="E15" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F15" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1333,16 +1309,16 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D16">
-        <v>0.5018518518518519</v>
+        <v>0.4948199948199948</v>
       </c>
       <c r="E16" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F16" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1353,16 +1329,16 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D17">
-        <v>0.4990740740740741</v>
+        <v>0.4877104377104377</v>
       </c>
       <c r="E17" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="F17" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1373,16 +1349,16 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D18">
-        <v>0.4948199948199948</v>
+        <v>0.4877104377104377</v>
       </c>
       <c r="E18" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F18" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1393,16 +1369,16 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D19">
-        <v>0.4877104377104377</v>
+        <v>0.4874125874125874</v>
       </c>
       <c r="E19" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F19" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1413,16 +1389,16 @@
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D20">
-        <v>0.4877104377104377</v>
+        <v>0.4796296296296296</v>
       </c>
       <c r="E20" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F20" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1433,16 +1409,16 @@
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D21">
-        <v>0.4874125874125874</v>
+        <v>0.4781144781144781</v>
       </c>
       <c r="E21" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F21" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -1453,16 +1429,16 @@
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D22">
-        <v>0.4796296296296296</v>
+        <v>0.477933177933178</v>
       </c>
       <c r="E22" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F22" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -1473,16 +1449,16 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D23">
-        <v>0.4781144781144781</v>
+        <v>0.4716931216931217</v>
       </c>
       <c r="E23" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F23" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1493,16 +1469,16 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D24">
-        <v>0.477933177933178</v>
+        <v>0.4707070707070707</v>
       </c>
       <c r="E24" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F24" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1513,16 +1489,16 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D25">
-        <v>0.4716931216931217</v>
+        <v>0.4681818181818182</v>
       </c>
       <c r="E25" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F25" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1533,16 +1509,16 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D26">
-        <v>0.4707070707070707</v>
+        <v>0.4681818181818182</v>
       </c>
       <c r="E26" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F26" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1553,16 +1529,16 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D27">
         <v>0.4681818181818182</v>
       </c>
       <c r="E27" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F27" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1573,16 +1549,16 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D28">
-        <v>0.4681818181818182</v>
+        <v>0.4671587671587671</v>
       </c>
       <c r="E28" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F28" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1593,16 +1569,16 @@
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D29">
-        <v>0.4681818181818182</v>
+        <v>0.4656565656565657</v>
       </c>
       <c r="E29" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F29" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1613,16 +1589,16 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D30">
-        <v>0.4671587671587671</v>
+        <v>0.4656565656565657</v>
       </c>
       <c r="E30" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F30" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1633,16 +1609,16 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D31">
-        <v>0.4656565656565657</v>
+        <v>0.4631313131313131</v>
       </c>
       <c r="E31" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F31" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1653,16 +1629,16 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D32">
-        <v>0.4656565656565657</v>
+        <v>0.462962962962963</v>
       </c>
       <c r="E32" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F32" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1673,16 +1649,16 @@
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D33">
-        <v>0.4631313131313131</v>
+        <v>0.4568181818181818</v>
       </c>
       <c r="E33" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F33" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1693,16 +1669,16 @@
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D34">
-        <v>0.462962962962963</v>
+        <v>0.4527972027972029</v>
       </c>
       <c r="E34" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F34" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1713,16 +1689,16 @@
         <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D35">
-        <v>0.4568181818181818</v>
+        <v>0.452020202020202</v>
       </c>
       <c r="E35" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="F35" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1733,16 +1709,16 @@
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D36">
-        <v>0.4527972027972029</v>
+        <v>0.452020202020202</v>
       </c>
       <c r="E36" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F36" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1753,16 +1729,16 @@
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D37">
-        <v>0.452020202020202</v>
+        <v>0.4478174603174603</v>
       </c>
       <c r="E37" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="F37" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1773,16 +1749,16 @@
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D38">
-        <v>0.452020202020202</v>
+        <v>0.442929292929293</v>
       </c>
       <c r="E38" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F38" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1793,16 +1769,16 @@
         <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D39">
-        <v>0.4478174603174603</v>
+        <v>0.442929292929293</v>
       </c>
       <c r="E39" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F39" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1813,16 +1789,16 @@
         <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D40">
-        <v>0.442929292929293</v>
+        <v>0.436026936026936</v>
       </c>
       <c r="E40" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F40" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1833,16 +1809,16 @@
         <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D41">
-        <v>0.442929292929293</v>
+        <v>0.4353535353535354</v>
       </c>
       <c r="E41" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F41" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1853,16 +1829,16 @@
         <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D42">
-        <v>0.436026936026936</v>
+        <v>0.4353535353535354</v>
       </c>
       <c r="E42" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F42" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1873,16 +1849,16 @@
         <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D43">
         <v>0.4353535353535354</v>
       </c>
       <c r="E43" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F43" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1893,16 +1869,16 @@
         <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D44">
-        <v>0.4353535353535354</v>
+        <v>0.4217171717171717</v>
       </c>
       <c r="E44" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F44" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1913,16 +1889,16 @@
         <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D45">
-        <v>0.4353535353535354</v>
+        <v>0.4217171717171717</v>
       </c>
       <c r="E45" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F45" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1933,16 +1909,16 @@
         <v>44</v>
       </c>
       <c r="C46" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D46">
-        <v>0.4217171717171717</v>
+        <v>0.4126262626262626</v>
       </c>
       <c r="E46" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F46" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1953,16 +1929,16 @@
         <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D47">
-        <v>0.4217171717171717</v>
+        <v>0.3918026418026417</v>
       </c>
       <c r="E47" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F47" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1973,16 +1949,16 @@
         <v>46</v>
       </c>
       <c r="C48" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D48">
-        <v>0.4126262626262626</v>
+        <v>0.3918026418026417</v>
       </c>
       <c r="E48" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F48" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1993,16 +1969,16 @@
         <v>47</v>
       </c>
       <c r="C49" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D49">
         <v>0.3918026418026417</v>
       </c>
       <c r="E49" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="F49" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -2013,16 +1989,16 @@
         <v>48</v>
       </c>
       <c r="C50" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D50">
         <v>0.3918026418026417</v>
       </c>
       <c r="E50" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F50" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2033,16 +2009,16 @@
         <v>49</v>
       </c>
       <c r="C51" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D51">
-        <v>0.3918026418026417</v>
+        <v>0.3851851851851851</v>
       </c>
       <c r="E51" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F51" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2053,16 +2029,16 @@
         <v>50</v>
       </c>
       <c r="C52" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D52">
-        <v>0.3918026418026417</v>
+        <v>0.3851851851851851</v>
       </c>
       <c r="E52" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F52" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -2073,16 +2049,16 @@
         <v>51</v>
       </c>
       <c r="C53" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D53">
         <v>0.3851851851851851</v>
       </c>
       <c r="E53" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="F53" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -2093,16 +2069,16 @@
         <v>52</v>
       </c>
       <c r="C54" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D54">
         <v>0.3851851851851851</v>
       </c>
       <c r="E54" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F54" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -2113,76 +2089,16 @@
         <v>53</v>
       </c>
       <c r="C55" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D55">
-        <v>0.3851851851851851</v>
+        <v>0.3606060606060606</v>
       </c>
       <c r="E55" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F55" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
-      <c r="A56" s="3">
-        <v>54</v>
-      </c>
-      <c r="B56" t="s">
-        <v>54</v>
-      </c>
-      <c r="C56" t="s">
-        <v>103</v>
-      </c>
-      <c r="D56">
-        <v>0.3851851851851851</v>
-      </c>
-      <c r="E56" t="s">
-        <v>151</v>
-      </c>
-      <c r="F56" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
-      <c r="A57" s="3">
-        <v>55</v>
-      </c>
-      <c r="B57" t="s">
-        <v>55</v>
-      </c>
-      <c r="C57" t="s">
-        <v>104</v>
-      </c>
-      <c r="D57">
-        <v>0.3606060606060606</v>
-      </c>
-      <c r="E57" t="s">
-        <v>152</v>
-      </c>
-      <c r="F57" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
-      <c r="A58" s="3">
-        <v>56</v>
-      </c>
-      <c r="B58" t="s">
-        <v>56</v>
-      </c>
-      <c r="C58" t="s">
-        <v>105</v>
-      </c>
-      <c r="D58">
-        <v>0.2526936026936027</v>
-      </c>
-      <c r="E58" t="s">
-        <v>153</v>
-      </c>
-      <c r="F58" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update similarity rating function with cosine similarity
</commit_message>
<xml_diff>
--- a/BackEnd/files/report.xlsx
+++ b/BackEnd/files/report.xlsx
@@ -7,139 +7,154 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="991001094847204574" sheetId="1" r:id="rId1"/>
+    <sheet name="991000001799704574" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="48">
-  <si>
-    <t>991001094847204574</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="54">
+  <si>
+    <t>991000001799704574</t>
+  </si>
+  <si>
+    <t>991000254419704574</t>
+  </si>
+  <si>
+    <t>991000121389704574</t>
   </si>
   <si>
     <t>991000252139704574</t>
   </si>
   <si>
-    <t>991000248959704574</t>
-  </si>
-  <si>
-    <t>991000099489704574</t>
-  </si>
-  <si>
-    <t>991000054469704574</t>
-  </si>
-  <si>
-    <t>991000360649704574</t>
-  </si>
-  <si>
-    <t>991000111639704574</t>
-  </si>
-  <si>
-    <t>991000243739704574</t>
-  </si>
-  <si>
-    <t>991000426459704574</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Children's edition of touching incidents and remarkable Answers to prayer </t>
+    <t>991000601979704574</t>
+  </si>
+  <si>
+    <t>991000050149704574</t>
+  </si>
+  <si>
+    <t>991000364949704574</t>
+  </si>
+  <si>
+    <t>991000250179704574</t>
+  </si>
+  <si>
+    <t>991000117479704574</t>
+  </si>
+  <si>
+    <t>991000576909704574</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Love and sex after 60 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sex, dating, and love </t>
+  </si>
+  <si>
+    <t>The sacred and profane love machine</t>
   </si>
   <si>
     <t xml:space="preserve">Free to love again </t>
   </si>
   <si>
-    <t xml:space="preserve">To mother with love </t>
-  </si>
-  <si>
-    <t xml:space="preserve">A light in the window </t>
-  </si>
-  <si>
-    <t>The love of learning and the desire for God</t>
-  </si>
-  <si>
-    <t xml:space="preserve">First things first </t>
-  </si>
-  <si>
-    <t xml:space="preserve">When families fight </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anthem </t>
+    <t xml:space="preserve">Middlemarch </t>
+  </si>
+  <si>
+    <t>Dangerous men &amp; adventurous women</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Double-header </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disney's Beauty and the beast </t>
+  </si>
+  <si>
+    <t>Disney's Beauty and the beast</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>['Christian life', 'Prayer', 'Children', 'Salvation', 'Christian life.', 'Children', 'Salvation.', 'Prayer.']</t>
+    <t>['Sex instruction for older people.', 'Older people', 'Love in old age.']</t>
+  </si>
+  <si>
+    <t>['Dating (Social customs)', 'Love.', 'Sex.']</t>
+  </si>
+  <si>
+    <t>['Man-woman relationships', 'Married people']</t>
   </si>
   <si>
     <t>['Sex', 'Christian life.']</t>
   </si>
   <si>
-    <t>['Christian poetry, American.', 'Poetry.']</t>
-  </si>
-  <si>
-    <t>['City and town life', 'Christian fiction.', 'Domestic fiction.']</t>
-  </si>
-  <si>
-    <t>['Monasticism and religious orders', 'Learning and scholarship', 'Christian literature, Early', 'Theology']</t>
-  </si>
-  <si>
-    <t>['Conduct of life.', 'Time management.']</t>
-  </si>
-  <si>
-    <t>['Family', 'Interpersonal conflict.', 'Life cycle, Human']</t>
-  </si>
-  <si>
-    <t>['Man-woman relationships', 'Men', 'Individuality', 'Time travel']</t>
-  </si>
-  <si>
-    <t>['christian', 'life', 'prayer', 'children', 'salvation']</t>
+    <t>['English.', 'City and town life', 'Married people', 'Young women', 'City and town life', 'Married people', 'Young women']</t>
+  </si>
+  <si>
+    <t>['Love stories, American', 'Women', 'Authors and readers', 'Love stories', 'Sex role in literature.']</t>
+  </si>
+  <si>
+    <t>['Monsters', 'Baseball', 'Early childhood education.', "Children's stories."]</t>
+  </si>
+  <si>
+    <t>['Early childhood education.', "Children's stories.", 'Fairy tales.', 'Folklore']</t>
+  </si>
+  <si>
+    <t>['Folklore.', 'Fairy tales.', 'Early childhood education.', "Children's stories."]</t>
+  </si>
+  <si>
+    <t>['sex', 'instruction', 'older', 'people', 'love', 'age']</t>
+  </si>
+  <si>
+    <t>['dating', 'social', 'customs', 'love', 'sex']</t>
+  </si>
+  <si>
+    <t>['man', 'woman', 'relationships', 'married', 'people']</t>
   </si>
   <si>
     <t>['sex', 'christian', 'life']</t>
   </si>
   <si>
-    <t>['christian', 'poetry', 'american']</t>
-  </si>
-  <si>
-    <t>['city', 'town', 'life', 'christian', 'fiction', 'domestic']</t>
-  </si>
-  <si>
-    <t>['monasticism', 'religious', 'orders', 'learning', 'christian', 'literature', 'early', 'theology']</t>
-  </si>
-  <si>
-    <t>['conduct', 'life', 'time', 'management']</t>
-  </si>
-  <si>
-    <t>['family', 'interpersonal', 'conflict', 'life', 'cycle', 'human']</t>
-  </si>
-  <si>
-    <t>['man', 'woman', 'relationships', 'men', 'individuality', 'time', 'travel']</t>
-  </si>
-  <si>
-    <t>[['christian', 'Christian'], ['life', 'living', 'animation', 'aliveness', 'lifetime', 'life-time', 'lifespan', 'liveliness', 'spirit', 'sprightliness', 'biography', 'life_story', 'life_history', 'life_sentence'], ['prayer', 'supplication', 'petition', 'orison', 'entreaty', 'appeal', 'supplicant'], ['children', 'child', 'kid', 'youngster', 'minor', 'shaver', 'nipper', 'small_fry', 'tiddler', 'tike', 'tyke', 'fry', 'nestling', 'baby'], ['salvation', 'redemption']]</t>
+    <t>['english', 'city', 'town', 'life', 'married', 'people', 'young', 'women']</t>
+  </si>
+  <si>
+    <t>['love', 'stories', 'american', 'women', 'authors', 'readers', 'sex', 'role', 'literature']</t>
+  </si>
+  <si>
+    <t>['monsters', 'baseball', 'early', 'childhood', 'education', 'children', 'stories']</t>
+  </si>
+  <si>
+    <t>['early', 'childhood', 'education', 'children', 'stories', 'fairy', 'tales', 'folklore']</t>
+  </si>
+  <si>
+    <t>['folklore', 'fairy', 'tales', 'early', 'childhood', 'education', 'children', 'stories']</t>
+  </si>
+  <si>
+    <t>[['sex', 'sexual_activity', 'sexual_practice', 'sex_activity', 'sexual_urge', 'gender', 'sexuality', 'arouse', 'excite', 'turn_on', 'wind_up'], ['instruction', 'direction', 'education', 'teaching', 'pedagogy', 'didactics', 'educational_activity', 'command', 'statement', 'program_line'], ['older', 'aged', 'elderly', 'senior', 'elder', 'sr.', 'old', 'erstwhile', 'former', 'onetime', 'one-time', 'quondam', 'sometime', 'honest-to-god', 'honest-to-goodness', 'sure-enough', 'Old', 'previous'], ['people', 'citizenry', 'multitude', 'masses', 'mass', 'hoi_polloi', 'the_great_unwashed'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['age', 'historic_period', 'eld', 'long_time', 'years', 'old_age', 'geezerhood', 'senesce', 'get_on', 'mature', 'maturate']]</t>
+  </si>
+  <si>
+    <t>[['dating', 'geological_dating', 'date', 'date_stamp', 'go_steady', 'go_out', 'see'], ['social', 'sociable', 'mixer', 'societal'], ['customs', 'customs_duty', 'custom', 'impost', 'usage', 'usance', 'tradition'], ['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['sex', 'sexual_activity', 'sexual_practice', 'sex_activity', 'sexual_urge', 'gender', 'sexuality', 'arouse', 'excite', 'turn_on', 'wind_up']]</t>
+  </si>
+  <si>
+    <t>[['man', 'adult_male', 'serviceman', 'military_man', 'military_personnel', 'homo', 'human_being', 'human', 'valet', 'valet_de_chambre', 'gentleman', "gentleman's_gentleman", 'Man', 'Isle_of_Man', 'piece', 'world', 'human_race', 'humanity', 'humankind', 'human_beings', 'humans', 'mankind'], ['woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['relationships', 'relationship', 'human_relationship', 'kinship', 'family_relationship'], ['married', 'marry', 'get_married', 'wed', 'conjoin', 'hook_up_with', 'get_hitched_with', 'espouse', 'tie', 'splice', 'marital', 'matrimonial'], ['people', 'citizenry', 'multitude', 'masses', 'mass', 'hoi_polloi', 'the_great_unwashed']]</t>
   </si>
   <si>
     <t>[['sex', 'sexual_activity', 'sexual_practice', 'sex_activity', 'sexual_urge', 'gender', 'sexuality', 'arouse', 'excite', 'turn_on', 'wind_up'], ['christian', 'Christian'], ['life', 'living', 'animation', 'aliveness', 'lifetime', 'life-time', 'lifespan', 'liveliness', 'spirit', 'sprightliness', 'biography', 'life_story', 'life_history', 'life_sentence']]</t>
   </si>
   <si>
-    <t>[['christian', 'Christian'], ['poetry', 'poesy', 'verse'], ['american', 'American', 'American_English', 'American_language']]</t>
-  </si>
-  <si>
-    <t>[['city', 'metropolis', 'urban_center'], ['town', 'townspeople', 'townsfolk', 'township', 'Town', 'Ithiel_Town'], ['life', 'living', 'animation', 'aliveness', 'lifetime', 'life-time', 'lifespan', 'liveliness', 'spirit', 'sprightliness', 'biography', 'life_story', 'life_history', 'life_sentence'], ['christian', 'Christian'], ['fiction', 'fabrication', 'fable'], ['domestic', 'domestic_help', 'house_servant', 'domesticated']]</t>
-  </si>
-  <si>
-    <t>[['monasticism'], ['religious', 'spiritual'], ['orders', 'order', 'order_of_magnitude', 'ordering', 'ordination', 'orderliness', 'decree', 'edict', 'fiat', 'rescript', 'purchase_order', 'club', 'social_club', 'society', 'guild', 'gild', 'lodge', 'rules_of_order', 'parliamentary_law', 'parliamentary_procedure', 'Holy_Order', 'Order', 'monastic_order', 'tell', 'enjoin', 'say', 'prescribe', 'dictate', 'regulate', 'regularize', 'regularise', 'govern', 'ordain', 'consecrate', 'ordinate', 'arrange', 'set_up', 'put', 'rate', 'rank', 'range', 'grade', 'place'], ['learning', 'acquisition', 'eruditeness', 'erudition', 'learnedness', 'scholarship', 'encyclopedism', 'encyclopaedism', 'learn', 'larn', 'acquire', 'hear', 'get_word', 'get_wind', 'pick_up', 'find_out', 'get_a_line', 'discover', 'see', 'memorize', 'memorise', 'con', 'study', 'read', 'take', 'teach', 'instruct', 'determine', 'check', 'ascertain', 'watch'], ['christian', 'Christian'], ['literature', 'lit'], ['early', 'former', 'other', 'early_on', 'ahead_of_time', 'too_soon', 'betimes'], ['theology', 'divinity', 'theological_system']]</t>
-  </si>
-  <si>
-    <t>[['conduct', 'behavior', 'behaviour', 'doings', 'demeanor', 'demeanour', 'deportment', 'carry_on', 'deal', 'lead', 'direct', 'behave', 'acquit', 'bear', 'deport', 'comport', 'carry', 'take', 'guide', 'impart', 'transmit', 'convey', 'channel'], ['life', 'living', 'animation', 'aliveness', 'lifetime', 'life-time', 'lifespan', 'liveliness', 'spirit', 'sprightliness', 'biography', 'life_story', 'life_history', 'life_sentence'], ['life', 'living', 'animation', 'aliveness', 'lifetime', 'life-time', 'lifespan', 'liveliness', 'spirit', 'sprightliness', 'biography', 'life_story', 'life_history', 'life_sentence'], ['management', 'direction']]</t>
-  </si>
-  <si>
-    <t>[['homes', 'home', 'place', 'dwelling', 'domicile', 'abode', 'habitation', 'dwelling_house', 'home_plate', 'home_base', 'plate', 'base', 'family', 'household', 'house', 'menage', 'nursing_home', 'rest_home'], ['interpersonal'], ['conflict', 'struggle', 'battle', 'fight', 'engagement', 'dispute', 'difference', 'difference_of_opinion', 'run_afoul', 'infringe', 'contravene'], ['life', 'living', 'animation', 'aliveness', 'lifetime', 'life-time', 'lifespan', 'liveliness', 'spirit', 'sprightliness', 'biography', 'life_story', 'life_history', 'life_sentence'], ['cycle', 'rhythm', 'round', 'hertz', 'Hz', 'cycle_per_second', 'cycles/second', 'cps', 'oscillation', 'bicycle', 'bike', 'wheel', 'motorbike', 'motorcycle', 'pedal'], ['man', 'adult_male', 'serviceman', 'military_man', 'military_personnel', 'homo', 'human_being', 'human', 'valet', 'valet_de_chambre', 'gentleman', "gentleman's_gentleman", 'Man', 'Isle_of_Man', 'piece', 'world', 'human_race', 'humanity', 'humankind', 'human_beings', 'humans', 'mankind']]</t>
-  </si>
-  <si>
-    <t>[['man', 'adult_male', 'serviceman', 'military_man', 'military_personnel', 'homo', 'human_being', 'human', 'valet', 'valet_de_chambre', 'gentleman', "gentleman's_gentleman", 'Man', 'Isle_of_Man', 'piece', 'world', 'human_race', 'humanity', 'humankind', 'human_beings', 'humans', 'mankind'], ['woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['relationships', 'relationship', 'human_relationship', 'kinship', 'family_relationship'], ['men', 'work_force', 'workforce', 'manpower', 'hands', 'man', 'adult_male', 'serviceman', 'military_man', 'military_personnel', 'homo', 'human_being', 'human', 'valet', 'valet_de_chambre', 'gentleman', "gentleman's_gentleman", 'Man', 'Isle_of_Man', 'piece', 'world', 'human_race', 'humanity', 'humankind', 'human_beings', 'humans', 'mankind'], ['identity', 'personal_identity', 'individuality', 'identity_element', 'identity_operator', 'identicalness', 'indistinguishability'], ['life', 'living', 'animation', 'aliveness', 'lifetime', 'life-time', 'lifespan', 'liveliness', 'spirit', 'sprightliness', 'biography', 'life_story', 'life_history', 'life_sentence'], ['travel', 'traveling', 'travelling', 'change_of_location', 'locomotion', 'go', 'move', 'locomote', 'journey', 'trip', 'jaunt', 'move_around']]</t>
+    <t>[['english', 'English', 'English_language', 'English_people', 'side'], ['city', 'metropolis', 'urban_center'], ['town', 'townspeople', 'townsfolk', 'township', 'Town', 'Ithiel_Town'], ['life', 'living', 'animation', 'aliveness', 'lifetime', 'life-time', 'lifespan', 'liveliness', 'spirit', 'sprightliness', 'biography', 'life_story', 'life_history', 'life_sentence'], ['married', 'marry', 'get_married', 'wed', 'conjoin', 'hook_up_with', 'get_hitched_with', 'espouse', 'tie', 'splice', 'marital', 'matrimonial'], ['people', 'citizenry', 'multitude', 'masses', 'mass', 'hoi_polloi', 'the_great_unwashed'], ['youth', 'young_person', 'younker', 'spring_chicken', 'young', 'early_days', 'youthfulness', 'juvenility'], ['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex']]</t>
+  </si>
+  <si>
+    <t>[['love', 'passion', 'beloved', 'dear', 'dearest', 'honey', 'sexual_love', 'erotic_love', 'lovemaking', 'making_love', 'love_life', 'enjoy', 'sleep_together', 'roll_in_the_hay', 'make_out', 'make_love', 'sleep_with', 'get_laid', 'have_sex', 'know', 'do_it', 'be_intimate', 'have_intercourse', 'have_it_away', 'have_it_off', 'screw', 'fuck', 'jazz', 'eff', 'hump', 'lie_with', 'bed', 'have_a_go_at_it', 'bang', 'get_it_on', 'bonk'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['american', 'American', 'American_English', 'American_language'], ['women', 'woman', 'adult_female', 'charwoman', 'char', 'cleaning_woman', 'cleaning_lady', 'womanhood', 'fair_sex'], ['authors', 'writer', 'author', 'generator', 'source'], ['readers', 'reader', 'subscriber', 'reviewer', 'referee', 'proofreader', 'lector', 'lecturer'], ['sex', 'sexual_activity', 'sexual_practice', 'sex_activity', 'sexual_urge', 'gender', 'sexuality', 'arouse', 'excite', 'turn_on', 'wind_up'], ['role', 'function', 'office', 'part', 'character', 'theatrical_role', 'persona', 'purpose', 'use'], ['literature', 'lit']]</t>
+  </si>
+  <si>
+    <t>[['monsters', 'monster', 'giant', 'goliath', 'behemoth', 'colossus', 'freak', 'monstrosity', 'lusus_naturae', 'fiend', 'devil', 'demon', 'ogre', 'teras'], ['baseball', 'baseball_game'], ['early', 'former', 'other', 'early_on', 'ahead_of_time', 'too_soon', 'betimes'], ['childhood', 'puerility'], ['instruction', 'direction', 'education', 'teaching', 'pedagogy', 'didactics', 'educational_activity', 'command', 'statement', 'program_line'], ['children', 'child', 'kid', 'youngster', 'minor', 'shaver', 'nipper', 'small_fry', 'tiddler', 'tike', 'tyke', 'fry', 'nestling', 'baby'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle']]</t>
+  </si>
+  <si>
+    <t>[['early', 'former', 'other', 'early_on', 'ahead_of_time', 'too_soon', 'betimes'], ['childhood', 'puerility'], ['instruction', 'direction', 'education', 'teaching', 'pedagogy', 'didactics', 'educational_activity', 'command', 'statement', 'program_line'], ['children', 'child', 'kid', 'youngster', 'minor', 'shaver', 'nipper', 'small_fry', 'tiddler', 'tike', 'tyke', 'fry', 'nestling', 'baby'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle'], ['fairy', 'faery', 'faerie', 'fay', 'sprite', 'fagot', 'faggot', 'fag', 'nance', 'pansy', 'queen', 'queer', 'poof', 'poove', 'pouf'], ['tales', 'narrative', 'narration', 'story', 'tale', 'fib', 'tarradiddle', 'taradiddle'], ['folklore']]</t>
+  </si>
+  <si>
+    <t>[['folklore'], ['fairy', 'faery', 'faerie', 'fay', 'sprite', 'fagot', 'faggot', 'fag', 'nance', 'pansy', 'queen', 'queer', 'poof', 'poove', 'pouf'], ['tales', 'narrative', 'narration', 'story', 'tale', 'fib', 'tarradiddle', 'taradiddle'], ['early', 'former', 'other', 'early_on', 'ahead_of_time', 'too_soon', 'betimes'], ['childhood', 'puerility'], ['instruction', 'direction', 'education', 'teaching', 'pedagogy', 'didactics', 'educational_activity', 'command', 'statement', 'program_line'], ['children', 'child', 'kid', 'youngster', 'minor', 'shaver', 'nipper', 'small_fry', 'tiddler', 'tike', 'tyke', 'fry', 'nestling', 'baby'], ['stories', 'narrative', 'narration', 'story', 'tale', 'floor', 'level', 'storey', 'history', 'account', 'chronicle', 'report', 'news_report', 'write_up', 'fib', 'tarradiddle', 'taradiddle']]</t>
   </si>
   <si>
     <t>Book ID</t>
@@ -154,7 +169,10 @@
     <t>Original Topics</t>
   </si>
   <si>
-    <t>Topics</t>
+    <t>Normalized Topics</t>
+  </si>
+  <si>
+    <t>Reduced Topics</t>
   </si>
   <si>
     <t>Synonyms</t>
@@ -541,41 +559,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
-    <col min="3" max="3" width="76.7109375" customWidth="1"/>
+    <col min="3" max="3" width="37.7109375" customWidth="1"/>
     <col min="4" max="4" width="7.7109375" customWidth="1"/>
-    <col min="5" max="5" width="111.7109375" customWidth="1"/>
-    <col min="6" max="6" width="100.7109375" customWidth="1"/>
-    <col min="7" max="7" width="1298.7109375" customWidth="1"/>
+    <col min="5" max="5" width="124.7109375" customWidth="1"/>
+    <col min="6" max="6" width="93.7109375" customWidth="1"/>
+    <col min="7" max="7" width="93.7109375" customWidth="1"/>
+    <col min="8" max="8" width="1229.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1">
+        <v>52</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -583,22 +605,25 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>29</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -606,22 +631,25 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>30</v>
+      </c>
+      <c r="H3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -629,22 +657,25 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>31</v>
+      </c>
+      <c r="H4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -652,22 +683,25 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>32</v>
+      </c>
+      <c r="H5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -675,22 +709,25 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D6">
         <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>33</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -698,22 +735,25 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D7">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>34</v>
+      </c>
+      <c r="H7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -721,22 +761,25 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D8">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s">
         <v>34</v>
       </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" t="s">
-        <v>31</v>
-      </c>
       <c r="G8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>34</v>
+      </c>
+      <c r="H8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -744,22 +787,25 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D9">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F9" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>35</v>
+      </c>
+      <c r="H9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -767,19 +813,48 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D10">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G10" t="s">
-        <v>41</v>
+        <v>36</v>
+      </c>
+      <c r="H10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11">
+        <v>23</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" t="s">
+        <v>37</v>
+      </c>
+      <c r="H11" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>